<commit_message>
feat：update new punch icon
</commit_message>
<xml_diff>
--- a/battleworld/Excel/MotionBtnData_技能按钮数据.xlsx
+++ b/battleworld/Excel/MotionBtnData_技能按钮数据.xlsx
@@ -8,12 +8,12 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
     </ext>
   </extLst>
 </workbook>
@@ -78,7 +78,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="微软雅黑"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">唯一</t>
@@ -88,7 +88,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">id</t>
@@ -106,7 +106,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="微软雅黑"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">是否显示</t>
@@ -116,7 +116,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">cd</t>
@@ -126,7 +126,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="微软雅黑"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">遮罩</t>
@@ -141,7 +141,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">0:1</t>
@@ -151,7 +151,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="微软雅黑"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">类型技能</t>
@@ -161,7 +161,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">id</t>
@@ -171,7 +171,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="微软雅黑"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">数组</t>
@@ -183,7 +183,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">1:3</t>
@@ -193,7 +193,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="微软雅黑"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">类型自动施放时间</t>
@@ -205,7 +205,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">1</t>
@@ -215,7 +215,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="微软雅黑"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">重击技能</t>
@@ -225,7 +225,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">id</t>
@@ -237,7 +237,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">1</t>
@@ -247,7 +247,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="微软雅黑"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">下落攻击</t>
@@ -257,7 +257,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">id</t>
@@ -269,7 +269,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">2</t>
@@ -279,7 +279,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="微软雅黑"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">事件名</t>
@@ -291,7 +291,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">2</t>
@@ -301,7 +301,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="微软雅黑"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">按钮</t>
@@ -311,7 +311,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">guid</t>
@@ -326,7 +326,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="微软雅黑"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">１：连击＋重击</t>
@@ -336,7 +336,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">+</t>
@@ -346,7 +346,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="微软雅黑"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">下落攻击</t>
@@ -358,7 +358,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">2:</t>
@@ -368,7 +368,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="微软雅黑"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">抬起、按下事件</t>
@@ -389,7 +389,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="微软雅黑"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">拳头普攻三连</t>
@@ -399,7 +399,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">+</t>
@@ -409,7 +409,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="微软雅黑"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">重击</t>
@@ -424,7 +424,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="微软雅黑"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">单手剑普攻三连</t>
@@ -434,7 +434,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">+</t>
@@ -444,7 +444,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="微软雅黑"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">重击</t>
@@ -459,7 +459,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="微软雅黑"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">法杖普攻二连</t>
@@ -469,7 +469,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">+</t>
@@ -479,7 +479,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="微软雅黑"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">重击</t>
@@ -494,7 +494,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="微软雅黑"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">拳头技能</t>
@@ -504,7 +504,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">1</t>
@@ -516,7 +516,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="微软雅黑"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">拳头技能</t>
@@ -526,7 +526,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">2</t>
@@ -538,7 +538,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="微软雅黑"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">拳头技能</t>
@@ -548,7 +548,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">3</t>
@@ -560,7 +560,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="微软雅黑"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">拳头技能</t>
@@ -570,7 +570,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">4</t>
@@ -582,7 +582,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="微软雅黑"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">拳头技能</t>
@@ -592,7 +592,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">5</t>
@@ -604,7 +604,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="微软雅黑"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">拳头技能</t>
@@ -614,7 +614,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">6</t>
@@ -626,7 +626,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="微软雅黑"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">拳头技能</t>
@@ -636,7 +636,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">7</t>
@@ -648,7 +648,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="微软雅黑"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">拳头技能</t>
@@ -658,7 +658,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">8</t>
@@ -670,7 +670,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="微软雅黑"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">拳头技能</t>
@@ -680,7 +680,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">9</t>
@@ -692,7 +692,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="微软雅黑"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">拳头技能</t>
@@ -702,7 +702,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">10</t>
@@ -714,7 +714,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="微软雅黑"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">单手剑技能</t>
@@ -724,7 +724,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">1</t>
@@ -736,7 +736,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="微软雅黑"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">单手剑技能</t>
@@ -746,7 +746,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">2</t>
@@ -758,7 +758,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="微软雅黑"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">单手剑技能</t>
@@ -768,7 +768,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">3</t>
@@ -780,7 +780,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="微软雅黑"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">单手剑技能</t>
@@ -790,7 +790,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">4</t>
@@ -802,7 +802,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="微软雅黑"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">单手剑技能</t>
@@ -812,7 +812,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">5</t>
@@ -824,7 +824,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="微软雅黑"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">单手剑技能</t>
@@ -834,7 +834,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">6</t>
@@ -846,7 +846,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="微软雅黑"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">单手剑技能</t>
@@ -856,7 +856,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">7</t>
@@ -868,7 +868,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="微软雅黑"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">单手剑技能</t>
@@ -878,7 +878,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">8</t>
@@ -890,7 +890,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="微软雅黑"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">单手剑技能</t>
@@ -900,7 +900,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">9</t>
@@ -912,7 +912,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="微软雅黑"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">单手剑技能</t>
@@ -922,7 +922,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">10</t>
@@ -934,7 +934,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="微软雅黑"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">法杖技能</t>
@@ -944,7 +944,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">1</t>
@@ -956,7 +956,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="微软雅黑"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">法杖技能</t>
@@ -966,7 +966,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">2</t>
@@ -978,7 +978,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="微软雅黑"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">法杖技能</t>
@@ -988,7 +988,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">3</t>
@@ -1000,7 +1000,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="微软雅黑"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">法杖技能</t>
@@ -1010,7 +1010,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">4</t>
@@ -1022,7 +1022,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="微软雅黑"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">法杖技能</t>
@@ -1032,7 +1032,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">5</t>
@@ -1044,7 +1044,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="微软雅黑"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">法杖技能</t>
@@ -1054,7 +1054,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">6</t>
@@ -1066,7 +1066,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="微软雅黑"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">法杖技能</t>
@@ -1076,7 +1076,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">7</t>
@@ -1088,7 +1088,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="微软雅黑"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">法杖技能</t>
@@ -1098,7 +1098,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">8</t>
@@ -1110,7 +1110,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="微软雅黑"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">法杖技能</t>
@@ -1120,7 +1120,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">9</t>
@@ -1132,7 +1132,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="微软雅黑"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">法杖技能</t>
@@ -1142,7 +1142,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">10</t>
@@ -1154,7 +1154,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="微软雅黑"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">双手剑普攻二连</t>
@@ -1164,7 +1164,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">+</t>
@@ -1174,7 +1174,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="微软雅黑"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">重击</t>
@@ -1189,7 +1189,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="微软雅黑"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">双手剑技能</t>
@@ -1199,7 +1199,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">1</t>
@@ -1211,7 +1211,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="微软雅黑"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">双手剑技能</t>
@@ -1221,7 +1221,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">2</t>
@@ -1233,7 +1233,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="微软雅黑"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">双手剑技能</t>
@@ -1243,7 +1243,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">3</t>
@@ -1255,7 +1255,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="微软雅黑"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">双手剑技能</t>
@@ -1265,7 +1265,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">4</t>
@@ -1277,7 +1277,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="微软雅黑"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">双手剑技能</t>
@@ -1287,7 +1287,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">5</t>
@@ -1299,7 +1299,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="微软雅黑"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">双手剑技能</t>
@@ -1309,7 +1309,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">6</t>
@@ -1321,7 +1321,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="微软雅黑"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">双手剑技能</t>
@@ -1331,7 +1331,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">7</t>
@@ -1343,7 +1343,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="微软雅黑"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">双手剑技能</t>
@@ -1353,7 +1353,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">8</t>
@@ -1365,7 +1365,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="微软雅黑"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">双手剑技能</t>
@@ -1375,7 +1375,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">9</t>
@@ -1387,7 +1387,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="微软雅黑"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">双手剑技能</t>
@@ -1397,7 +1397,7 @@
         <sz val="9.75"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">10</t>
@@ -1439,7 +1439,7 @@
     <font>
       <sz val="10"/>
       <name val="微软雅黑"/>
-      <family val="2"/>
+      <family val="0"/>
       <charset val="134"/>
     </font>
     <font>
@@ -1464,35 +1464,35 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="微软雅黑"/>
-      <family val="2"/>
+      <family val="0"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="9.75"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="9.75"/>
       <color rgb="FF000000"/>
       <name val="微软雅黑"/>
-      <family val="2"/>
+      <family val="0"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="9.8"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <family val="0"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -1562,7 +1562,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1584,15 +1584,11 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -1604,19 +1600,15 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -1628,7 +1620,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -1636,7 +1628,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -1648,10 +1640,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1664,6 +1660,18 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1739,6 +1747,178 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546a"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="e7e6e6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5b9bd5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ed7d31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a5a5a5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="ffc000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472c4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70ad47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563c1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954f72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" pitchFamily="0" charset="1"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" pitchFamily="0" charset="1"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+          <a:tileRect l="0" t="0" r="0" b="0"/>
+        </a:gradFill>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+          <a:tileRect l="0" t="0" r="0" b="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+          <a:tileRect l="0" t="0" r="0" b="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
@@ -1746,23 +1926,23 @@
   </sheetPr>
   <dimension ref="A1:T57"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="0" topLeftCell="F1" activePane="topRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="0" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="L9" activeCellId="0" sqref="L9"/>
+      <selection pane="topRight" activeCell="I21" activeCellId="0" sqref="I21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.0859375" defaultRowHeight="18.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.0859375" defaultRowHeight="16.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="1" width="30.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="44.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="44.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="39.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="30.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="21.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="31.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="27.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="11" style="1" width="11.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="27.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="11" style="1" width="11.21"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1981,7 +2161,7 @@
         <v>33</v>
       </c>
       <c r="K9" s="2" t="n">
-        <v>295458</v>
+        <v>325143</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2093,25 +2273,25 @@
       <c r="E13" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="F13" s="7" t="n">
+      <c r="F13" s="5" t="n">
         <v>17</v>
       </c>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="8"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
       <c r="K13" s="5" t="n">
         <v>295331</v>
       </c>
-      <c r="L13" s="9"/>
-      <c r="M13" s="9"/>
-      <c r="N13" s="9"/>
-      <c r="O13" s="9"/>
-      <c r="P13" s="9"/>
-      <c r="Q13" s="9"/>
-      <c r="R13" s="9"/>
-      <c r="S13" s="9"/>
-      <c r="T13" s="9"/>
+      <c r="L13" s="8"/>
+      <c r="M13" s="8"/>
+      <c r="N13" s="8"/>
+      <c r="O13" s="8"/>
+      <c r="P13" s="8"/>
+      <c r="Q13" s="8"/>
+      <c r="R13" s="8"/>
+      <c r="S13" s="8"/>
+      <c r="T13" s="8"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="n">
@@ -2129,25 +2309,25 @@
       <c r="E14" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="F14" s="7" t="n">
+      <c r="F14" s="5" t="n">
         <v>18</v>
       </c>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="8"/>
-      <c r="K14" s="10" t="n">
-        <v>295331</v>
-      </c>
-      <c r="L14" s="9"/>
-      <c r="M14" s="9"/>
-      <c r="N14" s="9"/>
-      <c r="O14" s="9"/>
-      <c r="P14" s="9"/>
-      <c r="Q14" s="9"/>
-      <c r="R14" s="9"/>
-      <c r="S14" s="9"/>
-      <c r="T14" s="9"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="9" t="n">
+        <v>325626</v>
+      </c>
+      <c r="L14" s="8"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="8"/>
+      <c r="O14" s="8"/>
+      <c r="P14" s="8"/>
+      <c r="Q14" s="8"/>
+      <c r="R14" s="8"/>
+      <c r="S14" s="8"/>
+      <c r="T14" s="8"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="5" t="n">
@@ -2165,25 +2345,25 @@
       <c r="E15" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="F15" s="7" t="n">
+      <c r="F15" s="5" t="n">
         <v>19</v>
       </c>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="8"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
       <c r="K15" s="5" t="n">
-        <v>295331</v>
-      </c>
-      <c r="L15" s="9"/>
-      <c r="M15" s="9"/>
-      <c r="N15" s="9"/>
-      <c r="O15" s="9"/>
-      <c r="P15" s="9"/>
-      <c r="Q15" s="9"/>
-      <c r="R15" s="9"/>
-      <c r="S15" s="9"/>
-      <c r="T15" s="9"/>
+        <v>325620</v>
+      </c>
+      <c r="L15" s="8"/>
+      <c r="M15" s="8"/>
+      <c r="N15" s="8"/>
+      <c r="O15" s="8"/>
+      <c r="P15" s="8"/>
+      <c r="Q15" s="8"/>
+      <c r="R15" s="8"/>
+      <c r="S15" s="8"/>
+      <c r="T15" s="8"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="5" t="n">
@@ -2201,25 +2381,25 @@
       <c r="E16" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="F16" s="7" t="n">
+      <c r="F16" s="5" t="n">
         <v>20</v>
       </c>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="10" t="n">
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="9" t="n">
         <v>295331</v>
       </c>
-      <c r="L16" s="9"/>
-      <c r="M16" s="9"/>
-      <c r="N16" s="9"/>
-      <c r="O16" s="9"/>
-      <c r="P16" s="9"/>
-      <c r="Q16" s="9"/>
-      <c r="R16" s="9"/>
-      <c r="S16" s="9"/>
-      <c r="T16" s="9"/>
+      <c r="L16" s="8"/>
+      <c r="M16" s="8"/>
+      <c r="N16" s="8"/>
+      <c r="O16" s="8"/>
+      <c r="P16" s="8"/>
+      <c r="Q16" s="8"/>
+      <c r="R16" s="8"/>
+      <c r="S16" s="8"/>
+      <c r="T16" s="8"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="5" t="n">
@@ -2237,25 +2417,25 @@
       <c r="E17" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="F17" s="7" t="n">
+      <c r="F17" s="5" t="n">
         <v>21</v>
       </c>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
-      <c r="I17" s="8"/>
-      <c r="J17" s="8"/>
-      <c r="K17" s="5" t="n">
-        <v>295331</v>
-      </c>
-      <c r="L17" s="9"/>
-      <c r="M17" s="9"/>
-      <c r="N17" s="9"/>
-      <c r="O17" s="9"/>
-      <c r="P17" s="9"/>
-      <c r="Q17" s="9"/>
-      <c r="R17" s="9"/>
-      <c r="S17" s="9"/>
-      <c r="T17" s="9"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="7"/>
+      <c r="J17" s="7"/>
+      <c r="K17" s="9" t="n">
+        <v>325614</v>
+      </c>
+      <c r="L17" s="8"/>
+      <c r="M17" s="8"/>
+      <c r="N17" s="8"/>
+      <c r="O17" s="8"/>
+      <c r="P17" s="8"/>
+      <c r="Q17" s="8"/>
+      <c r="R17" s="8"/>
+      <c r="S17" s="8"/>
+      <c r="T17" s="8"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="5" t="n">
@@ -2273,25 +2453,25 @@
       <c r="E18" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="F18" s="7" t="n">
+      <c r="F18" s="5" t="n">
         <v>22</v>
       </c>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="8"/>
-      <c r="J18" s="8"/>
-      <c r="K18" s="10" t="n">
-        <v>295331</v>
-      </c>
-      <c r="L18" s="9"/>
-      <c r="M18" s="9"/>
-      <c r="N18" s="9"/>
-      <c r="O18" s="9"/>
-      <c r="P18" s="9"/>
-      <c r="Q18" s="9"/>
-      <c r="R18" s="9"/>
-      <c r="S18" s="9"/>
-      <c r="T18" s="9"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="9" t="n">
+        <v>325605</v>
+      </c>
+      <c r="L18" s="8"/>
+      <c r="M18" s="8"/>
+      <c r="N18" s="8"/>
+      <c r="O18" s="8"/>
+      <c r="P18" s="8"/>
+      <c r="Q18" s="8"/>
+      <c r="R18" s="8"/>
+      <c r="S18" s="8"/>
+      <c r="T18" s="8"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="5" t="n">
@@ -2309,25 +2489,25 @@
       <c r="E19" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="F19" s="7" t="n">
+      <c r="F19" s="5" t="n">
         <v>23</v>
       </c>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
-      <c r="I19" s="8"/>
-      <c r="J19" s="8"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
       <c r="K19" s="5" t="n">
-        <v>295331</v>
-      </c>
-      <c r="L19" s="9"/>
-      <c r="M19" s="9"/>
-      <c r="N19" s="9"/>
-      <c r="O19" s="9"/>
-      <c r="P19" s="9"/>
-      <c r="Q19" s="9"/>
-      <c r="R19" s="9"/>
-      <c r="S19" s="9"/>
-      <c r="T19" s="9"/>
+        <v>325615</v>
+      </c>
+      <c r="L19" s="8"/>
+      <c r="M19" s="8"/>
+      <c r="N19" s="8"/>
+      <c r="O19" s="8"/>
+      <c r="P19" s="8"/>
+      <c r="Q19" s="8"/>
+      <c r="R19" s="8"/>
+      <c r="S19" s="8"/>
+      <c r="T19" s="8"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="5" t="n">
@@ -2345,25 +2525,25 @@
       <c r="E20" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="F20" s="7" t="n">
+      <c r="F20" s="5" t="n">
         <v>24</v>
       </c>
-      <c r="G20" s="8"/>
-      <c r="H20" s="8"/>
-      <c r="I20" s="8"/>
-      <c r="J20" s="8"/>
-      <c r="K20" s="10" t="n">
-        <v>295331</v>
-      </c>
-      <c r="L20" s="9"/>
-      <c r="M20" s="9"/>
-      <c r="N20" s="9"/>
-      <c r="O20" s="9"/>
-      <c r="P20" s="9"/>
-      <c r="Q20" s="9"/>
-      <c r="R20" s="9"/>
-      <c r="S20" s="9"/>
-      <c r="T20" s="9"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="9" t="n">
+        <v>325602</v>
+      </c>
+      <c r="L20" s="8"/>
+      <c r="M20" s="8"/>
+      <c r="N20" s="8"/>
+      <c r="O20" s="8"/>
+      <c r="P20" s="8"/>
+      <c r="Q20" s="8"/>
+      <c r="R20" s="8"/>
+      <c r="S20" s="8"/>
+      <c r="T20" s="8"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="5" t="n">
@@ -2381,25 +2561,25 @@
       <c r="E21" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="F21" s="7" t="n">
+      <c r="F21" s="5" t="n">
         <v>25</v>
       </c>
-      <c r="G21" s="8"/>
-      <c r="H21" s="8"/>
-      <c r="I21" s="8"/>
-      <c r="J21" s="8"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="7"/>
+      <c r="J21" s="7"/>
       <c r="K21" s="5" t="n">
-        <v>295331</v>
-      </c>
-      <c r="L21" s="9"/>
-      <c r="M21" s="9"/>
-      <c r="N21" s="9"/>
-      <c r="O21" s="9"/>
-      <c r="P21" s="9"/>
-      <c r="Q21" s="9"/>
-      <c r="R21" s="9"/>
-      <c r="S21" s="9"/>
-      <c r="T21" s="9"/>
+        <v>325612</v>
+      </c>
+      <c r="L21" s="8"/>
+      <c r="M21" s="8"/>
+      <c r="N21" s="8"/>
+      <c r="O21" s="8"/>
+      <c r="P21" s="8"/>
+      <c r="Q21" s="8"/>
+      <c r="R21" s="8"/>
+      <c r="S21" s="8"/>
+      <c r="T21" s="8"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="5" t="n">
@@ -2417,1145 +2597,1145 @@
       <c r="E22" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="F22" s="7" t="n">
+      <c r="F22" s="5" t="n">
         <v>26</v>
       </c>
-      <c r="G22" s="8"/>
-      <c r="H22" s="8"/>
-      <c r="I22" s="8"/>
-      <c r="J22" s="8"/>
-      <c r="K22" s="10" t="n">
-        <v>295331</v>
-      </c>
-      <c r="L22" s="9"/>
-      <c r="M22" s="9"/>
-      <c r="N22" s="9"/>
-      <c r="O22" s="9"/>
-      <c r="P22" s="9"/>
-      <c r="Q22" s="9"/>
-      <c r="R22" s="9"/>
-      <c r="S22" s="9"/>
-      <c r="T22" s="9"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
+      <c r="I22" s="7"/>
+      <c r="J22" s="7"/>
+      <c r="K22" s="9" t="n">
+        <v>325610</v>
+      </c>
+      <c r="L22" s="8"/>
+      <c r="M22" s="8"/>
+      <c r="N22" s="8"/>
+      <c r="O22" s="8"/>
+      <c r="P22" s="8"/>
+      <c r="Q22" s="8"/>
+      <c r="R22" s="8"/>
+      <c r="S22" s="8"/>
+      <c r="T22" s="8"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="11" t="n">
+      <c r="A23" s="10" t="n">
         <v>16</v>
       </c>
-      <c r="B23" s="12" t="s">
+      <c r="B23" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="C23" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="D23" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="E23" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="F23" s="13" t="n">
+      <c r="C23" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D23" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="E23" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F23" s="10" t="n">
         <v>27</v>
       </c>
-      <c r="G23" s="14"/>
-      <c r="H23" s="14"/>
-      <c r="I23" s="14"/>
-      <c r="J23" s="14"/>
-      <c r="K23" s="11" t="n">
+      <c r="G23" s="12"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="12"/>
+      <c r="J23" s="12"/>
+      <c r="K23" s="10" t="n">
         <v>294724</v>
       </c>
-      <c r="L23" s="15"/>
-      <c r="M23" s="15"/>
-      <c r="N23" s="15"/>
-      <c r="O23" s="15"/>
-      <c r="P23" s="15"/>
-      <c r="Q23" s="15"/>
-      <c r="R23" s="15"/>
-      <c r="S23" s="15"/>
-      <c r="T23" s="15"/>
+      <c r="L23" s="13"/>
+      <c r="M23" s="13"/>
+      <c r="N23" s="13"/>
+      <c r="O23" s="13"/>
+      <c r="P23" s="13"/>
+      <c r="Q23" s="13"/>
+      <c r="R23" s="13"/>
+      <c r="S23" s="13"/>
+      <c r="T23" s="13"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="11" t="n">
+      <c r="A24" s="10" t="n">
         <v>17</v>
       </c>
-      <c r="B24" s="12" t="s">
+      <c r="B24" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="C24" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="D24" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="E24" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="F24" s="13" t="n">
+      <c r="C24" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D24" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="E24" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F24" s="10" t="n">
         <v>28</v>
       </c>
-      <c r="G24" s="14"/>
-      <c r="H24" s="14"/>
-      <c r="I24" s="14"/>
-      <c r="J24" s="14"/>
-      <c r="K24" s="11" t="n">
+      <c r="G24" s="12"/>
+      <c r="H24" s="12"/>
+      <c r="I24" s="12"/>
+      <c r="J24" s="12"/>
+      <c r="K24" s="10" t="n">
         <v>294724</v>
       </c>
-      <c r="L24" s="15"/>
-      <c r="M24" s="15"/>
-      <c r="N24" s="15"/>
-      <c r="O24" s="15"/>
-      <c r="P24" s="15"/>
-      <c r="Q24" s="15"/>
-      <c r="R24" s="15"/>
-      <c r="S24" s="15"/>
-      <c r="T24" s="15"/>
+      <c r="L24" s="13"/>
+      <c r="M24" s="13"/>
+      <c r="N24" s="13"/>
+      <c r="O24" s="13"/>
+      <c r="P24" s="13"/>
+      <c r="Q24" s="13"/>
+      <c r="R24" s="13"/>
+      <c r="S24" s="13"/>
+      <c r="T24" s="13"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="11" t="n">
+      <c r="A25" s="10" t="n">
         <v>18</v>
       </c>
-      <c r="B25" s="12" t="s">
+      <c r="B25" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="C25" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="D25" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="E25" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="F25" s="13" t="n">
+      <c r="C25" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D25" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="E25" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F25" s="10" t="n">
         <v>29</v>
       </c>
-      <c r="G25" s="14"/>
-      <c r="H25" s="14"/>
-      <c r="I25" s="14"/>
-      <c r="J25" s="14"/>
-      <c r="K25" s="11" t="n">
+      <c r="G25" s="12"/>
+      <c r="H25" s="12"/>
+      <c r="I25" s="12"/>
+      <c r="J25" s="12"/>
+      <c r="K25" s="10" t="n">
         <v>294724</v>
       </c>
-      <c r="L25" s="15"/>
-      <c r="M25" s="15"/>
-      <c r="N25" s="15"/>
-      <c r="O25" s="15"/>
-      <c r="P25" s="15"/>
-      <c r="Q25" s="15"/>
-      <c r="R25" s="15"/>
-      <c r="S25" s="15"/>
-      <c r="T25" s="15"/>
+      <c r="L25" s="13"/>
+      <c r="M25" s="13"/>
+      <c r="N25" s="13"/>
+      <c r="O25" s="13"/>
+      <c r="P25" s="13"/>
+      <c r="Q25" s="13"/>
+      <c r="R25" s="13"/>
+      <c r="S25" s="13"/>
+      <c r="T25" s="13"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="11" t="n">
+      <c r="A26" s="10" t="n">
         <v>19</v>
       </c>
-      <c r="B26" s="12" t="s">
+      <c r="B26" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="C26" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="D26" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="E26" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="F26" s="13" t="n">
+      <c r="C26" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D26" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="E26" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F26" s="10" t="n">
         <v>30</v>
       </c>
-      <c r="G26" s="14"/>
-      <c r="H26" s="14"/>
-      <c r="I26" s="14"/>
-      <c r="J26" s="14"/>
-      <c r="K26" s="11" t="n">
+      <c r="G26" s="12"/>
+      <c r="H26" s="12"/>
+      <c r="I26" s="12"/>
+      <c r="J26" s="12"/>
+      <c r="K26" s="10" t="n">
         <v>294724</v>
       </c>
-      <c r="L26" s="15"/>
-      <c r="M26" s="15"/>
-      <c r="N26" s="15"/>
-      <c r="O26" s="15"/>
-      <c r="P26" s="15"/>
-      <c r="Q26" s="15"/>
-      <c r="R26" s="15"/>
-      <c r="S26" s="15"/>
-      <c r="T26" s="15"/>
+      <c r="L26" s="13"/>
+      <c r="M26" s="13"/>
+      <c r="N26" s="13"/>
+      <c r="O26" s="13"/>
+      <c r="P26" s="13"/>
+      <c r="Q26" s="13"/>
+      <c r="R26" s="13"/>
+      <c r="S26" s="13"/>
+      <c r="T26" s="13"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="11" t="n">
+      <c r="A27" s="10" t="n">
         <v>20</v>
       </c>
-      <c r="B27" s="12" t="s">
+      <c r="B27" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="C27" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="D27" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="E27" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="F27" s="13" t="n">
+      <c r="C27" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D27" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="E27" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F27" s="10" t="n">
         <v>31</v>
       </c>
-      <c r="G27" s="14"/>
-      <c r="H27" s="14"/>
-      <c r="I27" s="14"/>
-      <c r="J27" s="14"/>
-      <c r="K27" s="11" t="n">
+      <c r="G27" s="12"/>
+      <c r="H27" s="12"/>
+      <c r="I27" s="12"/>
+      <c r="J27" s="12"/>
+      <c r="K27" s="10" t="n">
         <v>294724</v>
       </c>
-      <c r="L27" s="15"/>
-      <c r="M27" s="15"/>
-      <c r="N27" s="15"/>
-      <c r="O27" s="15"/>
-      <c r="P27" s="15"/>
-      <c r="Q27" s="15"/>
-      <c r="R27" s="15"/>
-      <c r="S27" s="15"/>
-      <c r="T27" s="15"/>
+      <c r="L27" s="13"/>
+      <c r="M27" s="13"/>
+      <c r="N27" s="13"/>
+      <c r="O27" s="13"/>
+      <c r="P27" s="13"/>
+      <c r="Q27" s="13"/>
+      <c r="R27" s="13"/>
+      <c r="S27" s="13"/>
+      <c r="T27" s="13"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="11" t="n">
+      <c r="A28" s="10" t="n">
         <v>21</v>
       </c>
-      <c r="B28" s="12" t="s">
+      <c r="B28" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="C28" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="D28" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="E28" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="F28" s="13" t="n">
+      <c r="C28" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D28" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="E28" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F28" s="10" t="n">
         <v>32</v>
       </c>
-      <c r="G28" s="14"/>
-      <c r="H28" s="14"/>
-      <c r="I28" s="14"/>
-      <c r="J28" s="14"/>
-      <c r="K28" s="11" t="n">
+      <c r="G28" s="12"/>
+      <c r="H28" s="12"/>
+      <c r="I28" s="12"/>
+      <c r="J28" s="12"/>
+      <c r="K28" s="10" t="n">
         <v>294724</v>
       </c>
-      <c r="L28" s="15"/>
-      <c r="M28" s="15"/>
-      <c r="N28" s="15"/>
-      <c r="O28" s="15"/>
-      <c r="P28" s="15"/>
-      <c r="Q28" s="15"/>
-      <c r="R28" s="15"/>
-      <c r="S28" s="15"/>
-      <c r="T28" s="15"/>
+      <c r="L28" s="13"/>
+      <c r="M28" s="13"/>
+      <c r="N28" s="13"/>
+      <c r="O28" s="13"/>
+      <c r="P28" s="13"/>
+      <c r="Q28" s="13"/>
+      <c r="R28" s="13"/>
+      <c r="S28" s="13"/>
+      <c r="T28" s="13"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="11" t="n">
+      <c r="A29" s="10" t="n">
         <v>22</v>
       </c>
-      <c r="B29" s="12" t="s">
+      <c r="B29" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="C29" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="D29" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="E29" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="F29" s="13" t="n">
+      <c r="C29" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D29" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="E29" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F29" s="10" t="n">
         <v>33</v>
       </c>
-      <c r="G29" s="14"/>
-      <c r="H29" s="14"/>
-      <c r="I29" s="14"/>
-      <c r="J29" s="14"/>
-      <c r="K29" s="11" t="n">
+      <c r="G29" s="12"/>
+      <c r="H29" s="12"/>
+      <c r="I29" s="12"/>
+      <c r="J29" s="12"/>
+      <c r="K29" s="10" t="n">
         <v>294724</v>
       </c>
-      <c r="L29" s="15"/>
-      <c r="M29" s="15"/>
-      <c r="N29" s="15"/>
-      <c r="O29" s="15"/>
-      <c r="P29" s="15"/>
-      <c r="Q29" s="15"/>
-      <c r="R29" s="15"/>
-      <c r="S29" s="15"/>
-      <c r="T29" s="15"/>
+      <c r="L29" s="13"/>
+      <c r="M29" s="13"/>
+      <c r="N29" s="13"/>
+      <c r="O29" s="13"/>
+      <c r="P29" s="13"/>
+      <c r="Q29" s="13"/>
+      <c r="R29" s="13"/>
+      <c r="S29" s="13"/>
+      <c r="T29" s="13"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="11" t="n">
+      <c r="A30" s="10" t="n">
         <v>23</v>
       </c>
-      <c r="B30" s="12" t="s">
+      <c r="B30" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="C30" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="D30" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="E30" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="F30" s="13" t="n">
+      <c r="C30" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D30" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="E30" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F30" s="10" t="n">
         <v>34</v>
       </c>
-      <c r="G30" s="14"/>
-      <c r="H30" s="14"/>
-      <c r="I30" s="14"/>
-      <c r="J30" s="14"/>
-      <c r="K30" s="11" t="n">
+      <c r="G30" s="12"/>
+      <c r="H30" s="12"/>
+      <c r="I30" s="12"/>
+      <c r="J30" s="12"/>
+      <c r="K30" s="10" t="n">
         <v>294724</v>
       </c>
-      <c r="L30" s="15"/>
-      <c r="M30" s="15"/>
-      <c r="N30" s="15"/>
-      <c r="O30" s="15"/>
-      <c r="P30" s="15"/>
-      <c r="Q30" s="15"/>
-      <c r="R30" s="15"/>
-      <c r="S30" s="15"/>
-      <c r="T30" s="15"/>
+      <c r="L30" s="13"/>
+      <c r="M30" s="13"/>
+      <c r="N30" s="13"/>
+      <c r="O30" s="13"/>
+      <c r="P30" s="13"/>
+      <c r="Q30" s="13"/>
+      <c r="R30" s="13"/>
+      <c r="S30" s="13"/>
+      <c r="T30" s="13"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="11" t="n">
+      <c r="A31" s="10" t="n">
         <v>24</v>
       </c>
-      <c r="B31" s="12" t="s">
+      <c r="B31" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="C31" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="D31" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="E31" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="F31" s="13" t="n">
+      <c r="C31" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D31" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="E31" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F31" s="10" t="n">
         <v>35</v>
       </c>
-      <c r="G31" s="14"/>
-      <c r="H31" s="14"/>
-      <c r="I31" s="14"/>
-      <c r="J31" s="14"/>
-      <c r="K31" s="11" t="n">
+      <c r="G31" s="12"/>
+      <c r="H31" s="12"/>
+      <c r="I31" s="12"/>
+      <c r="J31" s="12"/>
+      <c r="K31" s="10" t="n">
         <v>294724</v>
       </c>
-      <c r="L31" s="15"/>
-      <c r="M31" s="15"/>
-      <c r="N31" s="15"/>
-      <c r="O31" s="15"/>
-      <c r="P31" s="15"/>
-      <c r="Q31" s="15"/>
-      <c r="R31" s="15"/>
-      <c r="S31" s="15"/>
-      <c r="T31" s="15"/>
+      <c r="L31" s="13"/>
+      <c r="M31" s="13"/>
+      <c r="N31" s="13"/>
+      <c r="O31" s="13"/>
+      <c r="P31" s="13"/>
+      <c r="Q31" s="13"/>
+      <c r="R31" s="13"/>
+      <c r="S31" s="13"/>
+      <c r="T31" s="13"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="11" t="n">
+      <c r="A32" s="10" t="n">
         <v>25</v>
       </c>
-      <c r="B32" s="12" t="s">
+      <c r="B32" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="C32" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="D32" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="E32" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="F32" s="13" t="n">
+      <c r="C32" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D32" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="E32" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F32" s="10" t="n">
         <v>36</v>
       </c>
-      <c r="G32" s="14"/>
-      <c r="H32" s="14"/>
-      <c r="I32" s="14"/>
-      <c r="J32" s="14"/>
-      <c r="K32" s="11" t="n">
+      <c r="G32" s="12"/>
+      <c r="H32" s="12"/>
+      <c r="I32" s="12"/>
+      <c r="J32" s="12"/>
+      <c r="K32" s="10" t="n">
         <v>294724</v>
       </c>
-      <c r="L32" s="15"/>
-      <c r="M32" s="15"/>
-      <c r="N32" s="15"/>
-      <c r="O32" s="15"/>
-      <c r="P32" s="15"/>
-      <c r="Q32" s="15"/>
-      <c r="R32" s="15"/>
-      <c r="S32" s="15"/>
-      <c r="T32" s="15"/>
+      <c r="L32" s="13"/>
+      <c r="M32" s="13"/>
+      <c r="N32" s="13"/>
+      <c r="O32" s="13"/>
+      <c r="P32" s="13"/>
+      <c r="Q32" s="13"/>
+      <c r="R32" s="13"/>
+      <c r="S32" s="13"/>
+      <c r="T32" s="13"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="16" t="n">
+      <c r="A33" s="14" t="n">
         <v>26</v>
       </c>
-      <c r="B33" s="17" t="s">
+      <c r="B33" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="C33" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="D33" s="16" t="n">
-        <v>1</v>
-      </c>
-      <c r="E33" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="F33" s="18" t="n">
+      <c r="C33" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="D33" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="E33" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="F33" s="16" t="n">
         <v>37</v>
       </c>
-      <c r="G33" s="19"/>
-      <c r="H33" s="19"/>
-      <c r="I33" s="19"/>
-      <c r="J33" s="19"/>
-      <c r="K33" s="16" t="n">
+      <c r="G33" s="17"/>
+      <c r="H33" s="17"/>
+      <c r="I33" s="17"/>
+      <c r="J33" s="17"/>
+      <c r="K33" s="14" t="n">
         <v>294753</v>
       </c>
-      <c r="L33" s="20"/>
-      <c r="M33" s="20"/>
-      <c r="N33" s="20"/>
-      <c r="O33" s="20"/>
-      <c r="P33" s="20"/>
-      <c r="Q33" s="20"/>
-      <c r="R33" s="20"/>
-      <c r="S33" s="20"/>
-      <c r="T33" s="20"/>
+      <c r="L33" s="18"/>
+      <c r="M33" s="18"/>
+      <c r="N33" s="18"/>
+      <c r="O33" s="18"/>
+      <c r="P33" s="18"/>
+      <c r="Q33" s="18"/>
+      <c r="R33" s="18"/>
+      <c r="S33" s="18"/>
+      <c r="T33" s="18"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="16" t="n">
+      <c r="A34" s="14" t="n">
         <v>27</v>
       </c>
-      <c r="B34" s="17" t="s">
+      <c r="B34" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="C34" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="D34" s="16" t="n">
-        <v>1</v>
-      </c>
-      <c r="E34" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="F34" s="18" t="n">
+      <c r="C34" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="D34" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="E34" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="F34" s="16" t="n">
         <v>38</v>
       </c>
-      <c r="G34" s="19"/>
-      <c r="H34" s="19"/>
-      <c r="I34" s="19"/>
-      <c r="J34" s="19"/>
-      <c r="K34" s="16" t="n">
+      <c r="G34" s="17"/>
+      <c r="H34" s="17"/>
+      <c r="I34" s="17"/>
+      <c r="J34" s="17"/>
+      <c r="K34" s="14" t="n">
         <v>294753</v>
       </c>
-      <c r="L34" s="20"/>
-      <c r="M34" s="20"/>
-      <c r="N34" s="20"/>
-      <c r="O34" s="20"/>
-      <c r="P34" s="20"/>
-      <c r="Q34" s="20"/>
-      <c r="R34" s="20"/>
-      <c r="S34" s="20"/>
-      <c r="T34" s="20"/>
+      <c r="L34" s="18"/>
+      <c r="M34" s="18"/>
+      <c r="N34" s="18"/>
+      <c r="O34" s="18"/>
+      <c r="P34" s="18"/>
+      <c r="Q34" s="18"/>
+      <c r="R34" s="18"/>
+      <c r="S34" s="18"/>
+      <c r="T34" s="18"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="16" t="n">
+      <c r="A35" s="14" t="n">
         <v>28</v>
       </c>
-      <c r="B35" s="17" t="s">
+      <c r="B35" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="C35" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="D35" s="16" t="n">
-        <v>1</v>
-      </c>
-      <c r="E35" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="F35" s="18" t="n">
+      <c r="C35" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="D35" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="E35" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="F35" s="16" t="n">
         <v>39</v>
       </c>
-      <c r="G35" s="19"/>
-      <c r="H35" s="19"/>
-      <c r="I35" s="19"/>
-      <c r="J35" s="19"/>
-      <c r="K35" s="16" t="n">
+      <c r="G35" s="17"/>
+      <c r="H35" s="17"/>
+      <c r="I35" s="17"/>
+      <c r="J35" s="17"/>
+      <c r="K35" s="14" t="n">
         <v>294753</v>
       </c>
-      <c r="L35" s="20"/>
-      <c r="M35" s="20"/>
-      <c r="N35" s="20"/>
-      <c r="O35" s="20"/>
-      <c r="P35" s="20"/>
-      <c r="Q35" s="20"/>
-      <c r="R35" s="20"/>
-      <c r="S35" s="20"/>
-      <c r="T35" s="20"/>
+      <c r="L35" s="18"/>
+      <c r="M35" s="18"/>
+      <c r="N35" s="18"/>
+      <c r="O35" s="18"/>
+      <c r="P35" s="18"/>
+      <c r="Q35" s="18"/>
+      <c r="R35" s="18"/>
+      <c r="S35" s="18"/>
+      <c r="T35" s="18"/>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="16" t="n">
+      <c r="A36" s="14" t="n">
         <v>29</v>
       </c>
-      <c r="B36" s="17" t="s">
+      <c r="B36" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="C36" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="D36" s="16" t="n">
-        <v>1</v>
-      </c>
-      <c r="E36" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="F36" s="18" t="n">
+      <c r="C36" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="D36" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="E36" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="F36" s="16" t="n">
         <v>40</v>
       </c>
-      <c r="G36" s="19"/>
-      <c r="H36" s="19"/>
-      <c r="I36" s="19"/>
-      <c r="J36" s="19"/>
-      <c r="K36" s="16" t="n">
+      <c r="G36" s="17"/>
+      <c r="H36" s="17"/>
+      <c r="I36" s="17"/>
+      <c r="J36" s="17"/>
+      <c r="K36" s="14" t="n">
         <v>294753</v>
       </c>
-      <c r="L36" s="20"/>
-      <c r="M36" s="20"/>
-      <c r="N36" s="20"/>
-      <c r="O36" s="20"/>
-      <c r="P36" s="20"/>
-      <c r="Q36" s="20"/>
-      <c r="R36" s="20"/>
-      <c r="S36" s="20"/>
-      <c r="T36" s="20"/>
+      <c r="L36" s="18"/>
+      <c r="M36" s="18"/>
+      <c r="N36" s="18"/>
+      <c r="O36" s="18"/>
+      <c r="P36" s="18"/>
+      <c r="Q36" s="18"/>
+      <c r="R36" s="18"/>
+      <c r="S36" s="18"/>
+      <c r="T36" s="18"/>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="16" t="n">
+      <c r="A37" s="14" t="n">
         <v>30</v>
       </c>
-      <c r="B37" s="17" t="s">
+      <c r="B37" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="C37" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="D37" s="16" t="n">
-        <v>1</v>
-      </c>
-      <c r="E37" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="F37" s="18" t="n">
+      <c r="C37" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="D37" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="E37" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="F37" s="16" t="n">
         <v>41</v>
       </c>
-      <c r="G37" s="19"/>
-      <c r="H37" s="19"/>
-      <c r="I37" s="19"/>
-      <c r="J37" s="19"/>
-      <c r="K37" s="16" t="n">
+      <c r="G37" s="17"/>
+      <c r="H37" s="17"/>
+      <c r="I37" s="17"/>
+      <c r="J37" s="17"/>
+      <c r="K37" s="14" t="n">
         <v>294753</v>
       </c>
-      <c r="L37" s="20"/>
-      <c r="M37" s="20"/>
-      <c r="N37" s="20"/>
-      <c r="O37" s="20"/>
-      <c r="P37" s="20"/>
-      <c r="Q37" s="20"/>
-      <c r="R37" s="20"/>
-      <c r="S37" s="20"/>
-      <c r="T37" s="20"/>
+      <c r="L37" s="18"/>
+      <c r="M37" s="18"/>
+      <c r="N37" s="18"/>
+      <c r="O37" s="18"/>
+      <c r="P37" s="18"/>
+      <c r="Q37" s="18"/>
+      <c r="R37" s="18"/>
+      <c r="S37" s="18"/>
+      <c r="T37" s="18"/>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="16" t="n">
+      <c r="A38" s="14" t="n">
         <v>31</v>
       </c>
-      <c r="B38" s="17" t="s">
+      <c r="B38" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="C38" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="D38" s="16" t="n">
-        <v>1</v>
-      </c>
-      <c r="E38" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="F38" s="18" t="n">
+      <c r="C38" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="D38" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="E38" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="F38" s="16" t="n">
         <v>42</v>
       </c>
-      <c r="G38" s="19"/>
-      <c r="H38" s="19"/>
-      <c r="I38" s="19"/>
-      <c r="J38" s="19"/>
-      <c r="K38" s="16" t="n">
+      <c r="G38" s="17"/>
+      <c r="H38" s="17"/>
+      <c r="I38" s="17"/>
+      <c r="J38" s="17"/>
+      <c r="K38" s="14" t="n">
         <v>294753</v>
       </c>
-      <c r="L38" s="20"/>
-      <c r="M38" s="20"/>
-      <c r="N38" s="20"/>
-      <c r="O38" s="20"/>
-      <c r="P38" s="20"/>
-      <c r="Q38" s="20"/>
-      <c r="R38" s="20"/>
-      <c r="S38" s="20"/>
-      <c r="T38" s="20"/>
+      <c r="L38" s="18"/>
+      <c r="M38" s="18"/>
+      <c r="N38" s="18"/>
+      <c r="O38" s="18"/>
+      <c r="P38" s="18"/>
+      <c r="Q38" s="18"/>
+      <c r="R38" s="18"/>
+      <c r="S38" s="18"/>
+      <c r="T38" s="18"/>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="16" t="n">
+      <c r="A39" s="14" t="n">
         <v>32</v>
       </c>
-      <c r="B39" s="17" t="s">
+      <c r="B39" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="C39" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="D39" s="16" t="n">
-        <v>1</v>
-      </c>
-      <c r="E39" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="F39" s="18" t="n">
+      <c r="C39" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="D39" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="E39" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="F39" s="16" t="n">
         <v>43</v>
       </c>
-      <c r="G39" s="19"/>
-      <c r="H39" s="19"/>
-      <c r="I39" s="19"/>
-      <c r="J39" s="19"/>
-      <c r="K39" s="16" t="n">
+      <c r="G39" s="17"/>
+      <c r="H39" s="17"/>
+      <c r="I39" s="17"/>
+      <c r="J39" s="17"/>
+      <c r="K39" s="14" t="n">
         <v>294753</v>
       </c>
-      <c r="L39" s="20"/>
-      <c r="M39" s="20"/>
-      <c r="N39" s="20"/>
-      <c r="O39" s="20"/>
-      <c r="P39" s="20"/>
-      <c r="Q39" s="20"/>
-      <c r="R39" s="20"/>
-      <c r="S39" s="20"/>
-      <c r="T39" s="20"/>
+      <c r="L39" s="18"/>
+      <c r="M39" s="18"/>
+      <c r="N39" s="18"/>
+      <c r="O39" s="18"/>
+      <c r="P39" s="18"/>
+      <c r="Q39" s="18"/>
+      <c r="R39" s="18"/>
+      <c r="S39" s="18"/>
+      <c r="T39" s="18"/>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="16" t="n">
+      <c r="A40" s="14" t="n">
         <v>33</v>
       </c>
-      <c r="B40" s="17" t="s">
+      <c r="B40" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="C40" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="D40" s="16" t="n">
-        <v>1</v>
-      </c>
-      <c r="E40" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="F40" s="18" t="n">
+      <c r="C40" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="D40" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="E40" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="F40" s="16" t="n">
         <v>44</v>
       </c>
-      <c r="G40" s="19"/>
-      <c r="H40" s="19"/>
-      <c r="I40" s="19"/>
-      <c r="J40" s="19"/>
-      <c r="K40" s="16" t="n">
+      <c r="G40" s="17"/>
+      <c r="H40" s="17"/>
+      <c r="I40" s="17"/>
+      <c r="J40" s="17"/>
+      <c r="K40" s="14" t="n">
         <v>294753</v>
       </c>
-      <c r="L40" s="20"/>
-      <c r="M40" s="20"/>
-      <c r="N40" s="20"/>
-      <c r="O40" s="20"/>
-      <c r="P40" s="20"/>
-      <c r="Q40" s="20"/>
-      <c r="R40" s="20"/>
-      <c r="S40" s="20"/>
-      <c r="T40" s="20"/>
+      <c r="L40" s="18"/>
+      <c r="M40" s="18"/>
+      <c r="N40" s="18"/>
+      <c r="O40" s="18"/>
+      <c r="P40" s="18"/>
+      <c r="Q40" s="18"/>
+      <c r="R40" s="18"/>
+      <c r="S40" s="18"/>
+      <c r="T40" s="18"/>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="16" t="n">
+      <c r="A41" s="14" t="n">
         <v>34</v>
       </c>
-      <c r="B41" s="17" t="s">
+      <c r="B41" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="C41" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="D41" s="16" t="n">
-        <v>1</v>
-      </c>
-      <c r="E41" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="F41" s="18" t="n">
+      <c r="C41" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="D41" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="E41" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="F41" s="16" t="n">
         <v>45</v>
       </c>
-      <c r="G41" s="19"/>
-      <c r="H41" s="19"/>
-      <c r="I41" s="19"/>
-      <c r="J41" s="19"/>
-      <c r="K41" s="16" t="n">
+      <c r="G41" s="17"/>
+      <c r="H41" s="17"/>
+      <c r="I41" s="17"/>
+      <c r="J41" s="17"/>
+      <c r="K41" s="14" t="n">
         <v>294753</v>
       </c>
-      <c r="L41" s="20"/>
-      <c r="M41" s="20"/>
-      <c r="N41" s="20"/>
-      <c r="O41" s="20"/>
-      <c r="P41" s="20"/>
-      <c r="Q41" s="20"/>
-      <c r="R41" s="20"/>
-      <c r="S41" s="20"/>
-      <c r="T41" s="20"/>
+      <c r="L41" s="18"/>
+      <c r="M41" s="18"/>
+      <c r="N41" s="18"/>
+      <c r="O41" s="18"/>
+      <c r="P41" s="18"/>
+      <c r="Q41" s="18"/>
+      <c r="R41" s="18"/>
+      <c r="S41" s="18"/>
+      <c r="T41" s="18"/>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="16" t="n">
+      <c r="A42" s="14" t="n">
         <v>35</v>
       </c>
-      <c r="B42" s="17" t="s">
+      <c r="B42" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="C42" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="D42" s="16" t="n">
-        <v>1</v>
-      </c>
-      <c r="E42" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="F42" s="18" t="n">
+      <c r="C42" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="D42" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="E42" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="F42" s="16" t="n">
         <v>46</v>
       </c>
-      <c r="G42" s="19"/>
-      <c r="H42" s="19"/>
-      <c r="I42" s="19"/>
-      <c r="J42" s="19"/>
-      <c r="K42" s="16" t="n">
+      <c r="G42" s="17"/>
+      <c r="H42" s="17"/>
+      <c r="I42" s="17"/>
+      <c r="J42" s="17"/>
+      <c r="K42" s="14" t="n">
         <v>294753</v>
       </c>
-      <c r="L42" s="20"/>
-      <c r="M42" s="20"/>
-      <c r="N42" s="20"/>
-      <c r="O42" s="20"/>
-      <c r="P42" s="20"/>
-      <c r="Q42" s="20"/>
-      <c r="R42" s="20"/>
-      <c r="S42" s="20"/>
-      <c r="T42" s="20"/>
+      <c r="L42" s="18"/>
+      <c r="M42" s="18"/>
+      <c r="N42" s="18"/>
+      <c r="O42" s="18"/>
+      <c r="P42" s="18"/>
+      <c r="Q42" s="18"/>
+      <c r="R42" s="18"/>
+      <c r="S42" s="18"/>
+      <c r="T42" s="18"/>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A43" s="21" t="n">
+      <c r="A43" s="19" t="n">
         <v>36</v>
       </c>
-      <c r="B43" s="22" t="s">
+      <c r="B43" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="C43" s="21" t="n">
-        <v>1</v>
-      </c>
-      <c r="D43" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="E43" s="21" t="n">
+      <c r="C43" s="19" t="n">
+        <v>1</v>
+      </c>
+      <c r="D43" s="19" t="n">
+        <v>0</v>
+      </c>
+      <c r="E43" s="19" t="n">
         <v>1</v>
       </c>
       <c r="F43" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="G43" s="23" t="n">
+      <c r="G43" s="22" t="n">
         <v>0.3</v>
       </c>
-      <c r="H43" s="23" t="n">
+      <c r="H43" s="22" t="n">
         <v>50</v>
       </c>
-      <c r="I43" s="23"/>
-      <c r="J43" s="21"/>
-      <c r="K43" s="21" t="n">
+      <c r="I43" s="22"/>
+      <c r="J43" s="19"/>
+      <c r="K43" s="19" t="n">
         <v>295273</v>
       </c>
-      <c r="L43" s="24"/>
-      <c r="M43" s="24"/>
-      <c r="N43" s="24"/>
-      <c r="O43" s="24"/>
-      <c r="P43" s="24"/>
-      <c r="Q43" s="24"/>
-      <c r="R43" s="24"/>
-      <c r="S43" s="24"/>
-      <c r="T43" s="24"/>
+      <c r="L43" s="23"/>
+      <c r="M43" s="23"/>
+      <c r="N43" s="23"/>
+      <c r="O43" s="23"/>
+      <c r="P43" s="23"/>
+      <c r="Q43" s="23"/>
+      <c r="R43" s="23"/>
+      <c r="S43" s="23"/>
+      <c r="T43" s="23"/>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A44" s="21" t="n">
+      <c r="A44" s="19" t="n">
         <v>37</v>
       </c>
-      <c r="B44" s="22" t="s">
+      <c r="B44" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="C44" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="D44" s="21" t="n">
-        <v>1</v>
-      </c>
-      <c r="E44" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="F44" s="25" t="n">
+      <c r="C44" s="19" t="n">
+        <v>0</v>
+      </c>
+      <c r="D44" s="19" t="n">
+        <v>1</v>
+      </c>
+      <c r="E44" s="19" t="n">
+        <v>0</v>
+      </c>
+      <c r="F44" s="24" t="n">
         <v>51</v>
       </c>
-      <c r="G44" s="23"/>
-      <c r="H44" s="23"/>
-      <c r="I44" s="23"/>
-      <c r="J44" s="23"/>
-      <c r="K44" s="21" t="n">
+      <c r="G44" s="22"/>
+      <c r="H44" s="22"/>
+      <c r="I44" s="22"/>
+      <c r="J44" s="22"/>
+      <c r="K44" s="19" t="n">
         <v>295345</v>
       </c>
-      <c r="L44" s="24"/>
-      <c r="M44" s="24"/>
-      <c r="N44" s="24"/>
-      <c r="O44" s="24"/>
-      <c r="P44" s="24"/>
-      <c r="Q44" s="24"/>
-      <c r="R44" s="24"/>
-      <c r="S44" s="24"/>
-      <c r="T44" s="24"/>
+      <c r="L44" s="23"/>
+      <c r="M44" s="23"/>
+      <c r="N44" s="23"/>
+      <c r="O44" s="23"/>
+      <c r="P44" s="23"/>
+      <c r="Q44" s="23"/>
+      <c r="R44" s="23"/>
+      <c r="S44" s="23"/>
+      <c r="T44" s="23"/>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="21" t="n">
+      <c r="A45" s="19" t="n">
         <v>38</v>
       </c>
-      <c r="B45" s="22" t="s">
+      <c r="B45" s="20" t="s">
         <v>73</v>
       </c>
-      <c r="C45" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="D45" s="21" t="n">
-        <v>1</v>
-      </c>
-      <c r="E45" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="F45" s="25" t="n">
+      <c r="C45" s="19" t="n">
+        <v>0</v>
+      </c>
+      <c r="D45" s="19" t="n">
+        <v>1</v>
+      </c>
+      <c r="E45" s="19" t="n">
+        <v>0</v>
+      </c>
+      <c r="F45" s="24" t="n">
         <v>52</v>
       </c>
-      <c r="G45" s="23"/>
-      <c r="H45" s="23"/>
-      <c r="I45" s="23"/>
-      <c r="J45" s="23"/>
-      <c r="K45" s="21" t="n">
+      <c r="G45" s="22"/>
+      <c r="H45" s="22"/>
+      <c r="I45" s="22"/>
+      <c r="J45" s="22"/>
+      <c r="K45" s="19" t="n">
         <v>295345</v>
       </c>
-      <c r="L45" s="24"/>
-      <c r="M45" s="24"/>
-      <c r="N45" s="24"/>
-      <c r="O45" s="24"/>
-      <c r="P45" s="24"/>
-      <c r="Q45" s="24"/>
-      <c r="R45" s="24"/>
-      <c r="S45" s="24"/>
-      <c r="T45" s="24"/>
+      <c r="L45" s="23"/>
+      <c r="M45" s="23"/>
+      <c r="N45" s="23"/>
+      <c r="O45" s="23"/>
+      <c r="P45" s="23"/>
+      <c r="Q45" s="23"/>
+      <c r="R45" s="23"/>
+      <c r="S45" s="23"/>
+      <c r="T45" s="23"/>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A46" s="21" t="n">
+      <c r="A46" s="19" t="n">
         <v>39</v>
       </c>
-      <c r="B46" s="22" t="s">
+      <c r="B46" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="C46" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="D46" s="21" t="n">
-        <v>1</v>
-      </c>
-      <c r="E46" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="F46" s="25" t="n">
+      <c r="C46" s="19" t="n">
+        <v>0</v>
+      </c>
+      <c r="D46" s="19" t="n">
+        <v>1</v>
+      </c>
+      <c r="E46" s="19" t="n">
+        <v>0</v>
+      </c>
+      <c r="F46" s="24" t="n">
         <v>53</v>
       </c>
-      <c r="G46" s="23"/>
-      <c r="H46" s="23"/>
-      <c r="I46" s="23"/>
-      <c r="J46" s="23"/>
-      <c r="K46" s="21" t="n">
+      <c r="G46" s="22"/>
+      <c r="H46" s="22"/>
+      <c r="I46" s="22"/>
+      <c r="J46" s="22"/>
+      <c r="K46" s="19" t="n">
         <v>295345</v>
       </c>
-      <c r="L46" s="24"/>
-      <c r="M46" s="24"/>
-      <c r="N46" s="24"/>
-      <c r="O46" s="24"/>
-      <c r="P46" s="24"/>
-      <c r="Q46" s="24"/>
-      <c r="R46" s="24"/>
-      <c r="S46" s="24"/>
-      <c r="T46" s="24"/>
+      <c r="L46" s="23"/>
+      <c r="M46" s="23"/>
+      <c r="N46" s="23"/>
+      <c r="O46" s="23"/>
+      <c r="P46" s="23"/>
+      <c r="Q46" s="23"/>
+      <c r="R46" s="23"/>
+      <c r="S46" s="23"/>
+      <c r="T46" s="23"/>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A47" s="21" t="n">
+      <c r="A47" s="19" t="n">
         <v>40</v>
       </c>
-      <c r="B47" s="22" t="s">
+      <c r="B47" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="C47" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="D47" s="21" t="n">
-        <v>1</v>
-      </c>
-      <c r="E47" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="F47" s="25" t="n">
+      <c r="C47" s="19" t="n">
+        <v>0</v>
+      </c>
+      <c r="D47" s="19" t="n">
+        <v>1</v>
+      </c>
+      <c r="E47" s="19" t="n">
+        <v>0</v>
+      </c>
+      <c r="F47" s="24" t="n">
         <v>54</v>
       </c>
-      <c r="G47" s="23"/>
-      <c r="H47" s="23"/>
-      <c r="I47" s="23"/>
-      <c r="J47" s="23"/>
-      <c r="K47" s="21" t="n">
+      <c r="G47" s="22"/>
+      <c r="H47" s="22"/>
+      <c r="I47" s="22"/>
+      <c r="J47" s="22"/>
+      <c r="K47" s="19" t="n">
         <v>295345</v>
       </c>
-      <c r="L47" s="24"/>
-      <c r="M47" s="24"/>
-      <c r="N47" s="24"/>
-      <c r="O47" s="24"/>
-      <c r="P47" s="24"/>
-      <c r="Q47" s="24"/>
-      <c r="R47" s="24"/>
-      <c r="S47" s="24"/>
-      <c r="T47" s="24"/>
+      <c r="L47" s="23"/>
+      <c r="M47" s="23"/>
+      <c r="N47" s="23"/>
+      <c r="O47" s="23"/>
+      <c r="P47" s="23"/>
+      <c r="Q47" s="23"/>
+      <c r="R47" s="23"/>
+      <c r="S47" s="23"/>
+      <c r="T47" s="23"/>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A48" s="21" t="n">
+      <c r="A48" s="19" t="n">
         <v>41</v>
       </c>
-      <c r="B48" s="22" t="s">
+      <c r="B48" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="C48" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="D48" s="21" t="n">
-        <v>1</v>
-      </c>
-      <c r="E48" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="F48" s="25" t="n">
+      <c r="C48" s="19" t="n">
+        <v>0</v>
+      </c>
+      <c r="D48" s="19" t="n">
+        <v>1</v>
+      </c>
+      <c r="E48" s="19" t="n">
+        <v>0</v>
+      </c>
+      <c r="F48" s="24" t="n">
         <v>55</v>
       </c>
-      <c r="G48" s="23"/>
-      <c r="H48" s="23"/>
-      <c r="I48" s="23"/>
-      <c r="J48" s="23"/>
-      <c r="K48" s="21" t="n">
+      <c r="G48" s="22"/>
+      <c r="H48" s="22"/>
+      <c r="I48" s="22"/>
+      <c r="J48" s="22"/>
+      <c r="K48" s="19" t="n">
         <v>295345</v>
       </c>
-      <c r="L48" s="24"/>
-      <c r="M48" s="24"/>
-      <c r="N48" s="24"/>
-      <c r="O48" s="24"/>
-      <c r="P48" s="24"/>
-      <c r="Q48" s="24"/>
-      <c r="R48" s="24"/>
-      <c r="S48" s="24"/>
-      <c r="T48" s="24"/>
+      <c r="L48" s="23"/>
+      <c r="M48" s="23"/>
+      <c r="N48" s="23"/>
+      <c r="O48" s="23"/>
+      <c r="P48" s="23"/>
+      <c r="Q48" s="23"/>
+      <c r="R48" s="23"/>
+      <c r="S48" s="23"/>
+      <c r="T48" s="23"/>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A49" s="21" t="n">
+      <c r="A49" s="19" t="n">
         <v>42</v>
       </c>
-      <c r="B49" s="22" t="s">
+      <c r="B49" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="C49" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="D49" s="21" t="n">
-        <v>1</v>
-      </c>
-      <c r="E49" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="F49" s="25" t="n">
+      <c r="C49" s="19" t="n">
+        <v>0</v>
+      </c>
+      <c r="D49" s="19" t="n">
+        <v>1</v>
+      </c>
+      <c r="E49" s="19" t="n">
+        <v>0</v>
+      </c>
+      <c r="F49" s="24" t="n">
         <v>56</v>
       </c>
-      <c r="G49" s="23"/>
-      <c r="H49" s="23"/>
-      <c r="I49" s="23"/>
-      <c r="J49" s="23"/>
-      <c r="K49" s="21" t="n">
+      <c r="G49" s="22"/>
+      <c r="H49" s="22"/>
+      <c r="I49" s="22"/>
+      <c r="J49" s="22"/>
+      <c r="K49" s="19" t="n">
         <v>295345</v>
       </c>
-      <c r="L49" s="24"/>
-      <c r="M49" s="24"/>
-      <c r="N49" s="24"/>
-      <c r="O49" s="24"/>
-      <c r="P49" s="24"/>
-      <c r="Q49" s="24"/>
-      <c r="R49" s="24"/>
-      <c r="S49" s="24"/>
-      <c r="T49" s="24"/>
+      <c r="L49" s="23"/>
+      <c r="M49" s="23"/>
+      <c r="N49" s="23"/>
+      <c r="O49" s="23"/>
+      <c r="P49" s="23"/>
+      <c r="Q49" s="23"/>
+      <c r="R49" s="23"/>
+      <c r="S49" s="23"/>
+      <c r="T49" s="23"/>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A50" s="21" t="n">
+      <c r="A50" s="19" t="n">
         <v>43</v>
       </c>
-      <c r="B50" s="22" t="s">
+      <c r="B50" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="C50" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="D50" s="21" t="n">
-        <v>1</v>
-      </c>
-      <c r="E50" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="F50" s="25" t="n">
+      <c r="C50" s="19" t="n">
+        <v>0</v>
+      </c>
+      <c r="D50" s="19" t="n">
+        <v>1</v>
+      </c>
+      <c r="E50" s="19" t="n">
+        <v>0</v>
+      </c>
+      <c r="F50" s="24" t="n">
         <v>57</v>
       </c>
-      <c r="G50" s="23"/>
-      <c r="H50" s="23"/>
-      <c r="I50" s="23"/>
-      <c r="J50" s="23"/>
-      <c r="K50" s="21" t="n">
+      <c r="G50" s="22"/>
+      <c r="H50" s="22"/>
+      <c r="I50" s="22"/>
+      <c r="J50" s="22"/>
+      <c r="K50" s="19" t="n">
         <v>295345</v>
       </c>
-      <c r="L50" s="24"/>
-      <c r="M50" s="24"/>
-      <c r="N50" s="24"/>
-      <c r="O50" s="24"/>
-      <c r="P50" s="24"/>
-      <c r="Q50" s="24"/>
-      <c r="R50" s="24"/>
-      <c r="S50" s="24"/>
-      <c r="T50" s="24"/>
+      <c r="L50" s="23"/>
+      <c r="M50" s="23"/>
+      <c r="N50" s="23"/>
+      <c r="O50" s="23"/>
+      <c r="P50" s="23"/>
+      <c r="Q50" s="23"/>
+      <c r="R50" s="23"/>
+      <c r="S50" s="23"/>
+      <c r="T50" s="23"/>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A51" s="21" t="n">
+      <c r="A51" s="19" t="n">
         <v>44</v>
       </c>
-      <c r="B51" s="22" t="s">
+      <c r="B51" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="C51" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="D51" s="21" t="n">
-        <v>1</v>
-      </c>
-      <c r="E51" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="F51" s="25" t="n">
+      <c r="C51" s="19" t="n">
+        <v>0</v>
+      </c>
+      <c r="D51" s="19" t="n">
+        <v>1</v>
+      </c>
+      <c r="E51" s="19" t="n">
+        <v>0</v>
+      </c>
+      <c r="F51" s="24" t="n">
         <v>58</v>
       </c>
-      <c r="G51" s="23"/>
-      <c r="H51" s="23"/>
-      <c r="I51" s="23"/>
-      <c r="J51" s="23"/>
-      <c r="K51" s="21" t="n">
+      <c r="G51" s="22"/>
+      <c r="H51" s="22"/>
+      <c r="I51" s="22"/>
+      <c r="J51" s="22"/>
+      <c r="K51" s="19" t="n">
         <v>295345</v>
       </c>
-      <c r="L51" s="24"/>
-      <c r="M51" s="24"/>
-      <c r="N51" s="24"/>
-      <c r="O51" s="24"/>
-      <c r="P51" s="24"/>
-      <c r="Q51" s="24"/>
-      <c r="R51" s="24"/>
-      <c r="S51" s="24"/>
-      <c r="T51" s="24"/>
+      <c r="L51" s="23"/>
+      <c r="M51" s="23"/>
+      <c r="N51" s="23"/>
+      <c r="O51" s="23"/>
+      <c r="P51" s="23"/>
+      <c r="Q51" s="23"/>
+      <c r="R51" s="23"/>
+      <c r="S51" s="23"/>
+      <c r="T51" s="23"/>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A52" s="21" t="n">
+      <c r="A52" s="19" t="n">
         <v>45</v>
       </c>
-      <c r="B52" s="22" t="s">
+      <c r="B52" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="C52" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="D52" s="21" t="n">
-        <v>1</v>
-      </c>
-      <c r="E52" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="F52" s="25" t="n">
+      <c r="C52" s="19" t="n">
+        <v>0</v>
+      </c>
+      <c r="D52" s="19" t="n">
+        <v>1</v>
+      </c>
+      <c r="E52" s="19" t="n">
+        <v>0</v>
+      </c>
+      <c r="F52" s="24" t="n">
         <v>59</v>
       </c>
-      <c r="G52" s="23"/>
-      <c r="H52" s="23"/>
-      <c r="I52" s="23"/>
-      <c r="J52" s="23"/>
-      <c r="K52" s="21" t="n">
+      <c r="G52" s="22"/>
+      <c r="H52" s="22"/>
+      <c r="I52" s="22"/>
+      <c r="J52" s="22"/>
+      <c r="K52" s="19" t="n">
         <v>295345</v>
       </c>
-      <c r="L52" s="24"/>
-      <c r="M52" s="24"/>
-      <c r="N52" s="24"/>
-      <c r="O52" s="24"/>
-      <c r="P52" s="24"/>
-      <c r="Q52" s="24"/>
-      <c r="R52" s="24"/>
-      <c r="S52" s="24"/>
-      <c r="T52" s="24"/>
+      <c r="L52" s="23"/>
+      <c r="M52" s="23"/>
+      <c r="N52" s="23"/>
+      <c r="O52" s="23"/>
+      <c r="P52" s="23"/>
+      <c r="Q52" s="23"/>
+      <c r="R52" s="23"/>
+      <c r="S52" s="23"/>
+      <c r="T52" s="23"/>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A53" s="21" t="n">
+      <c r="A53" s="19" t="n">
         <v>46</v>
       </c>
-      <c r="B53" s="22" t="s">
+      <c r="B53" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="C53" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="D53" s="21" t="n">
-        <v>1</v>
-      </c>
-      <c r="E53" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="F53" s="25" t="n">
+      <c r="C53" s="19" t="n">
+        <v>0</v>
+      </c>
+      <c r="D53" s="19" t="n">
+        <v>1</v>
+      </c>
+      <c r="E53" s="19" t="n">
+        <v>0</v>
+      </c>
+      <c r="F53" s="24" t="n">
         <v>60</v>
       </c>
-      <c r="G53" s="23"/>
-      <c r="H53" s="23"/>
-      <c r="I53" s="23"/>
-      <c r="J53" s="23"/>
-      <c r="K53" s="21" t="n">
+      <c r="G53" s="22"/>
+      <c r="H53" s="22"/>
+      <c r="I53" s="22"/>
+      <c r="J53" s="22"/>
+      <c r="K53" s="19" t="n">
         <v>295345</v>
       </c>
-      <c r="L53" s="24"/>
-      <c r="M53" s="24"/>
-      <c r="N53" s="24"/>
-      <c r="O53" s="24"/>
-      <c r="P53" s="24"/>
-      <c r="Q53" s="24"/>
-      <c r="R53" s="24"/>
-      <c r="S53" s="24"/>
-      <c r="T53" s="24"/>
+      <c r="L53" s="23"/>
+      <c r="M53" s="23"/>
+      <c r="N53" s="23"/>
+      <c r="O53" s="23"/>
+      <c r="P53" s="23"/>
+      <c r="Q53" s="23"/>
+      <c r="R53" s="23"/>
+      <c r="S53" s="23"/>
+      <c r="T53" s="23"/>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="5" t="n">
@@ -3573,133 +3753,133 @@
       <c r="E54" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="F54" s="5" t="s">
+      <c r="F54" s="25" t="s">
         <v>83</v>
       </c>
-      <c r="G54" s="8"/>
-      <c r="H54" s="8"/>
-      <c r="I54" s="8"/>
+      <c r="G54" s="7"/>
+      <c r="H54" s="7"/>
+      <c r="I54" s="7"/>
       <c r="J54" s="5"/>
       <c r="K54" s="5" t="n">
         <v>295281</v>
       </c>
-      <c r="L54" s="9"/>
-      <c r="M54" s="9"/>
-      <c r="N54" s="9"/>
-      <c r="O54" s="9"/>
-      <c r="P54" s="9"/>
-      <c r="Q54" s="9"/>
-      <c r="R54" s="9"/>
-      <c r="S54" s="9"/>
-      <c r="T54" s="9"/>
+      <c r="L54" s="8"/>
+      <c r="M54" s="8"/>
+      <c r="N54" s="8"/>
+      <c r="O54" s="8"/>
+      <c r="P54" s="8"/>
+      <c r="Q54" s="8"/>
+      <c r="R54" s="8"/>
+      <c r="S54" s="8"/>
+      <c r="T54" s="8"/>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A55" s="11" t="n">
+      <c r="A55" s="10" t="n">
         <v>48</v>
       </c>
-      <c r="B55" s="12" t="s">
+      <c r="B55" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="C55" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="D55" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="E55" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="F55" s="11" t="s">
+      <c r="C55" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D55" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E55" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="F55" s="26" t="s">
         <v>85</v>
       </c>
-      <c r="G55" s="14"/>
-      <c r="H55" s="14"/>
-      <c r="I55" s="14"/>
-      <c r="J55" s="11"/>
-      <c r="K55" s="11" t="n">
+      <c r="G55" s="12"/>
+      <c r="H55" s="12"/>
+      <c r="I55" s="12"/>
+      <c r="J55" s="10"/>
+      <c r="K55" s="10" t="n">
         <v>295344</v>
       </c>
-      <c r="L55" s="15"/>
-      <c r="M55" s="15"/>
-      <c r="N55" s="15"/>
-      <c r="O55" s="15"/>
-      <c r="P55" s="15"/>
-      <c r="Q55" s="15"/>
-      <c r="R55" s="15"/>
-      <c r="S55" s="15"/>
-      <c r="T55" s="15"/>
+      <c r="L55" s="13"/>
+      <c r="M55" s="13"/>
+      <c r="N55" s="13"/>
+      <c r="O55" s="13"/>
+      <c r="P55" s="13"/>
+      <c r="Q55" s="13"/>
+      <c r="R55" s="13"/>
+      <c r="S55" s="13"/>
+      <c r="T55" s="13"/>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A56" s="16" t="n">
+      <c r="A56" s="14" t="n">
         <v>49</v>
       </c>
-      <c r="B56" s="17" t="s">
+      <c r="B56" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="C56" s="16" t="n">
-        <v>1</v>
-      </c>
-      <c r="D56" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="E56" s="16" t="n">
-        <v>1</v>
-      </c>
-      <c r="F56" s="16" t="s">
+      <c r="C56" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="D56" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="E56" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="F56" s="27" t="s">
         <v>87</v>
       </c>
-      <c r="G56" s="19"/>
-      <c r="H56" s="19"/>
-      <c r="I56" s="19"/>
-      <c r="J56" s="16"/>
-      <c r="K56" s="16" t="n">
+      <c r="G56" s="17"/>
+      <c r="H56" s="17"/>
+      <c r="I56" s="17"/>
+      <c r="J56" s="14"/>
+      <c r="K56" s="14" t="n">
         <v>295287</v>
       </c>
-      <c r="L56" s="20"/>
-      <c r="M56" s="20"/>
-      <c r="N56" s="20"/>
-      <c r="O56" s="20"/>
-      <c r="P56" s="20"/>
-      <c r="Q56" s="20"/>
-      <c r="R56" s="20"/>
-      <c r="S56" s="20"/>
-      <c r="T56" s="20"/>
+      <c r="L56" s="18"/>
+      <c r="M56" s="18"/>
+      <c r="N56" s="18"/>
+      <c r="O56" s="18"/>
+      <c r="P56" s="18"/>
+      <c r="Q56" s="18"/>
+      <c r="R56" s="18"/>
+      <c r="S56" s="18"/>
+      <c r="T56" s="18"/>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A57" s="21" t="n">
+      <c r="A57" s="19" t="n">
         <v>50</v>
       </c>
-      <c r="B57" s="22" t="s">
+      <c r="B57" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="C57" s="21" t="n">
-        <v>1</v>
-      </c>
-      <c r="D57" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="E57" s="21" t="n">
+      <c r="C57" s="19" t="n">
+        <v>1</v>
+      </c>
+      <c r="D57" s="19" t="n">
+        <v>0</v>
+      </c>
+      <c r="E57" s="19" t="n">
         <v>1</v>
       </c>
       <c r="F57" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="G57" s="23"/>
-      <c r="H57" s="23"/>
-      <c r="I57" s="23"/>
-      <c r="J57" s="21"/>
-      <c r="K57" s="21" t="n">
+      <c r="G57" s="22"/>
+      <c r="H57" s="22"/>
+      <c r="I57" s="22"/>
+      <c r="J57" s="19"/>
+      <c r="K57" s="19" t="n">
         <v>295273</v>
       </c>
-      <c r="L57" s="24"/>
-      <c r="M57" s="24"/>
-      <c r="N57" s="24"/>
-      <c r="O57" s="24"/>
-      <c r="P57" s="24"/>
-      <c r="Q57" s="24"/>
-      <c r="R57" s="24"/>
-      <c r="S57" s="24"/>
-      <c r="T57" s="24"/>
+      <c r="L57" s="23"/>
+      <c r="M57" s="23"/>
+      <c r="N57" s="23"/>
+      <c r="O57" s="23"/>
+      <c r="P57" s="23"/>
+      <c r="Q57" s="23"/>
+      <c r="R57" s="23"/>
+      <c r="S57" s="23"/>
+      <c r="T57" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="10">

</xml_diff>

<commit_message>
feat：update new excel change
</commit_message>
<xml_diff>
--- a/battleworld/Excel/MotionBtnData_技能按钮数据.xlsx
+++ b/battleworld/Excel/MotionBtnData_技能按钮数据.xlsx
@@ -1927,9 +1927,9 @@
   <dimension ref="A1:T57"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="0" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <pane xSplit="2" ySplit="0" topLeftCell="E1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="I21" activeCellId="0" sqref="I21"/>
+      <selection pane="topRight" activeCell="G25" activeCellId="0" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.0859375" defaultRowHeight="16.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2281,7 +2281,7 @@
       <c r="I13" s="7"/>
       <c r="J13" s="7"/>
       <c r="K13" s="5" t="n">
-        <v>295331</v>
+        <v>337389</v>
       </c>
       <c r="L13" s="8"/>
       <c r="M13" s="8"/>
@@ -2641,7 +2641,7 @@
       <c r="I23" s="12"/>
       <c r="J23" s="12"/>
       <c r="K23" s="10" t="n">
-        <v>294724</v>
+        <v>326706</v>
       </c>
       <c r="L23" s="13"/>
       <c r="M23" s="13"/>
@@ -2677,7 +2677,7 @@
       <c r="I24" s="12"/>
       <c r="J24" s="12"/>
       <c r="K24" s="10" t="n">
-        <v>294724</v>
+        <v>326704</v>
       </c>
       <c r="L24" s="13"/>
       <c r="M24" s="13"/>
@@ -2713,7 +2713,7 @@
       <c r="I25" s="12"/>
       <c r="J25" s="12"/>
       <c r="K25" s="10" t="n">
-        <v>294724</v>
+        <v>326705</v>
       </c>
       <c r="L25" s="13"/>
       <c r="M25" s="13"/>
@@ -2785,7 +2785,7 @@
       <c r="I27" s="12"/>
       <c r="J27" s="12"/>
       <c r="K27" s="10" t="n">
-        <v>294724</v>
+        <v>326710</v>
       </c>
       <c r="L27" s="13"/>
       <c r="M27" s="13"/>
@@ -2821,7 +2821,7 @@
       <c r="I28" s="12"/>
       <c r="J28" s="12"/>
       <c r="K28" s="10" t="n">
-        <v>294724</v>
+        <v>327113</v>
       </c>
       <c r="L28" s="13"/>
       <c r="M28" s="13"/>
@@ -2857,7 +2857,7 @@
       <c r="I29" s="12"/>
       <c r="J29" s="12"/>
       <c r="K29" s="10" t="n">
-        <v>294724</v>
+        <v>326693</v>
       </c>
       <c r="L29" s="13"/>
       <c r="M29" s="13"/>
@@ -2893,7 +2893,7 @@
       <c r="I30" s="12"/>
       <c r="J30" s="12"/>
       <c r="K30" s="10" t="n">
-        <v>294724</v>
+        <v>326698</v>
       </c>
       <c r="L30" s="13"/>
       <c r="M30" s="13"/>
@@ -2929,7 +2929,7 @@
       <c r="I31" s="12"/>
       <c r="J31" s="12"/>
       <c r="K31" s="10" t="n">
-        <v>294724</v>
+        <v>326699</v>
       </c>
       <c r="L31" s="13"/>
       <c r="M31" s="13"/>
@@ -2965,7 +2965,7 @@
       <c r="I32" s="12"/>
       <c r="J32" s="12"/>
       <c r="K32" s="10" t="n">
-        <v>294724</v>
+        <v>326712</v>
       </c>
       <c r="L32" s="13"/>
       <c r="M32" s="13"/>
@@ -3001,7 +3001,7 @@
       <c r="I33" s="17"/>
       <c r="J33" s="17"/>
       <c r="K33" s="14" t="n">
-        <v>294753</v>
+        <v>327119</v>
       </c>
       <c r="L33" s="18"/>
       <c r="M33" s="18"/>
@@ -3073,7 +3073,7 @@
       <c r="I35" s="17"/>
       <c r="J35" s="17"/>
       <c r="K35" s="14" t="n">
-        <v>294753</v>
+        <v>327136</v>
       </c>
       <c r="L35" s="18"/>
       <c r="M35" s="18"/>
@@ -3109,7 +3109,7 @@
       <c r="I36" s="17"/>
       <c r="J36" s="17"/>
       <c r="K36" s="14" t="n">
-        <v>294753</v>
+        <v>327101</v>
       </c>
       <c r="L36" s="18"/>
       <c r="M36" s="18"/>
@@ -3181,7 +3181,7 @@
       <c r="I38" s="17"/>
       <c r="J38" s="17"/>
       <c r="K38" s="14" t="n">
-        <v>294753</v>
+        <v>327099</v>
       </c>
       <c r="L38" s="18"/>
       <c r="M38" s="18"/>
@@ -3217,7 +3217,7 @@
       <c r="I39" s="17"/>
       <c r="J39" s="17"/>
       <c r="K39" s="14" t="n">
-        <v>294753</v>
+        <v>327118</v>
       </c>
       <c r="L39" s="18"/>
       <c r="M39" s="18"/>
@@ -3253,7 +3253,7 @@
       <c r="I40" s="17"/>
       <c r="J40" s="17"/>
       <c r="K40" s="14" t="n">
-        <v>294753</v>
+        <v>327099</v>
       </c>
       <c r="L40" s="18"/>
       <c r="M40" s="18"/>
@@ -3289,7 +3289,7 @@
       <c r="I41" s="17"/>
       <c r="J41" s="17"/>
       <c r="K41" s="14" t="n">
-        <v>294753</v>
+        <v>327126</v>
       </c>
       <c r="L41" s="18"/>
       <c r="M41" s="18"/>
@@ -3325,7 +3325,7 @@
       <c r="I42" s="17"/>
       <c r="J42" s="17"/>
       <c r="K42" s="14" t="n">
-        <v>294753</v>
+        <v>327104</v>
       </c>
       <c r="L42" s="18"/>
       <c r="M42" s="18"/>
@@ -3401,7 +3401,7 @@
       <c r="I44" s="22"/>
       <c r="J44" s="22"/>
       <c r="K44" s="19" t="n">
-        <v>295345</v>
+        <v>327083</v>
       </c>
       <c r="L44" s="23"/>
       <c r="M44" s="23"/>
@@ -3437,7 +3437,7 @@
       <c r="I45" s="22"/>
       <c r="J45" s="22"/>
       <c r="K45" s="19" t="n">
-        <v>295345</v>
+        <v>327089</v>
       </c>
       <c r="L45" s="23"/>
       <c r="M45" s="23"/>
@@ -3509,7 +3509,7 @@
       <c r="I47" s="22"/>
       <c r="J47" s="22"/>
       <c r="K47" s="19" t="n">
-        <v>295345</v>
+        <v>327088</v>
       </c>
       <c r="L47" s="23"/>
       <c r="M47" s="23"/>
@@ -3545,7 +3545,7 @@
       <c r="I48" s="22"/>
       <c r="J48" s="22"/>
       <c r="K48" s="19" t="n">
-        <v>295345</v>
+        <v>327087</v>
       </c>
       <c r="L48" s="23"/>
       <c r="M48" s="23"/>
@@ -3581,7 +3581,7 @@
       <c r="I49" s="22"/>
       <c r="J49" s="22"/>
       <c r="K49" s="19" t="n">
-        <v>295345</v>
+        <v>327170</v>
       </c>
       <c r="L49" s="23"/>
       <c r="M49" s="23"/>
@@ -3617,7 +3617,7 @@
       <c r="I50" s="22"/>
       <c r="J50" s="22"/>
       <c r="K50" s="19" t="n">
-        <v>295345</v>
+        <v>327094</v>
       </c>
       <c r="L50" s="23"/>
       <c r="M50" s="23"/>
@@ -3653,7 +3653,7 @@
       <c r="I51" s="22"/>
       <c r="J51" s="22"/>
       <c r="K51" s="19" t="n">
-        <v>295345</v>
+        <v>327171</v>
       </c>
       <c r="L51" s="23"/>
       <c r="M51" s="23"/>
@@ -3689,7 +3689,7 @@
       <c r="I52" s="22"/>
       <c r="J52" s="22"/>
       <c r="K52" s="19" t="n">
-        <v>295345</v>
+        <v>327097</v>
       </c>
       <c r="L52" s="23"/>
       <c r="M52" s="23"/>
@@ -3725,7 +3725,7 @@
       <c r="I53" s="22"/>
       <c r="J53" s="22"/>
       <c r="K53" s="19" t="n">
-        <v>295345</v>
+        <v>327100</v>
       </c>
       <c r="L53" s="23"/>
       <c r="M53" s="23"/>

</xml_diff>

<commit_message>
feat：update new excel of skill icon
</commit_message>
<xml_diff>
--- a/battleworld/Excel/MotionBtnData_技能按钮数据.xlsx
+++ b/battleworld/Excel/MotionBtnData_技能按钮数据.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="130">
   <si>
     <t xml:space="preserve">int</t>
   </si>
@@ -511,6 +511,9 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">四方震击√</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="9.75"/>
@@ -533,6 +536,9 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">地脉震动√</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="9.75"/>
@@ -555,6 +561,9 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">引力冲击√</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="9.75"/>
@@ -577,6 +586,9 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">蓄力冲拳√</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="9.75"/>
@@ -599,6 +611,9 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">震地空爆√</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="9.75"/>
@@ -621,6 +636,9 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">战吼√</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="9.75"/>
@@ -643,6 +661,9 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">洪雷震爆√</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="9.75"/>
@@ -665,6 +686,9 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">升龙冲拳√</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="9.75"/>
@@ -687,6 +711,9 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">狂风聚集√</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="9.75"/>
@@ -709,6 +736,9 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">原力涌动√</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="9.75"/>
@@ -731,6 +761,9 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">洪雷剑气√</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="9.75"/>
@@ -753,6 +786,9 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">雷霆轰击√</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="9.75"/>
@@ -775,6 +811,9 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">燕返√</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="9.75"/>
@@ -797,6 +836,9 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">巨雷一击√</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="9.75"/>
@@ -819,6 +861,9 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">千鸟√</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="9.75"/>
@@ -841,6 +886,9 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">引雷√</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="9.75"/>
@@ -863,6 +911,9 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">雷霆连斩√</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="9.75"/>
@@ -885,6 +936,9 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">引雷入体√</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="9.75"/>
@@ -907,6 +961,9 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">聚雷阵√</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="9.75"/>
@@ -929,6 +986,9 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">雷切√</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="9.75"/>
@@ -951,6 +1011,9 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">光明降临√</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="9.75"/>
@@ -973,6 +1036,9 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">光之冲击√</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="9.75"/>
@@ -995,6 +1061,9 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">炫光一闪√</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="9.75"/>
@@ -1017,6 +1086,9 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">光明疗愈√</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="9.75"/>
@@ -1039,6 +1111,9 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">光之飞弹√</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="9.75"/>
@@ -1061,6 +1136,9 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">时光禁锢√</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="9.75"/>
@@ -1083,6 +1161,9 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">圣炎领域√</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="9.75"/>
@@ -1105,6 +1186,9 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">聚能光炮√</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="9.75"/>
@@ -1127,6 +1211,9 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">光之庇护√</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="9.75"/>
@@ -1149,6 +1236,9 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">光焰附魔√</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="9.75"/>
@@ -1206,6 +1296,9 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">烈焰突刺√</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="9.75"/>
@@ -1228,6 +1321,9 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">旋风斩击√</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="9.75"/>
@@ -1250,6 +1346,9 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">爆炎重击√</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="9.75"/>
@@ -1272,6 +1371,9 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">火雨√</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="9.75"/>
@@ -1294,6 +1396,9 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">烈焰飞劈√</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="9.75"/>
@@ -1316,6 +1421,9 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">巨焰剑气√</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="9.75"/>
@@ -1338,6 +1446,9 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">竖劈√</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="9.75"/>
@@ -1360,6 +1471,9 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">飞凰突击√</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="9.75"/>
@@ -1382,6 +1496,9 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">火焰庇护√</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="9.75"/>
@@ -1402,6 +1519,9 @@
       </rPr>
       <t xml:space="preserve">10</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">焰能觉醒√</t>
   </si>
   <si>
     <t xml:space="preserve">拳头怒气普攻</t>
@@ -1926,10 +2046,10 @@
   </sheetPr>
   <dimension ref="A1:T57"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="0" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="G25" activeCellId="0" sqref="G25"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="0" topLeftCell="K31" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A31" activeCellId="0" sqref="A31"/>
+      <selection pane="topRight" activeCell="L51" activeCellId="0" sqref="L51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.0859375" defaultRowHeight="16.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2281,9 +2401,11 @@
       <c r="I13" s="7"/>
       <c r="J13" s="7"/>
       <c r="K13" s="5" t="n">
-        <v>337389</v>
-      </c>
-      <c r="L13" s="8"/>
+        <v>350390</v>
+      </c>
+      <c r="L13" s="8" t="s">
+        <v>41</v>
+      </c>
       <c r="M13" s="8"/>
       <c r="N13" s="8"/>
       <c r="O13" s="8"/>
@@ -2298,7 +2420,7 @@
         <v>7</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C14" s="5" t="n">
         <v>0</v>
@@ -2317,9 +2439,11 @@
       <c r="I14" s="7"/>
       <c r="J14" s="7"/>
       <c r="K14" s="9" t="n">
-        <v>325626</v>
-      </c>
-      <c r="L14" s="8"/>
+        <v>350378</v>
+      </c>
+      <c r="L14" s="8" t="s">
+        <v>43</v>
+      </c>
       <c r="M14" s="8"/>
       <c r="N14" s="8"/>
       <c r="O14" s="8"/>
@@ -2334,7 +2458,7 @@
         <v>8</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C15" s="5" t="n">
         <v>0</v>
@@ -2353,9 +2477,11 @@
       <c r="I15" s="7"/>
       <c r="J15" s="7"/>
       <c r="K15" s="5" t="n">
-        <v>325620</v>
-      </c>
-      <c r="L15" s="8"/>
+        <v>350359</v>
+      </c>
+      <c r="L15" s="8" t="s">
+        <v>45</v>
+      </c>
       <c r="M15" s="8"/>
       <c r="N15" s="8"/>
       <c r="O15" s="8"/>
@@ -2370,7 +2496,7 @@
         <v>9</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C16" s="5" t="n">
         <v>0</v>
@@ -2389,9 +2515,11 @@
       <c r="I16" s="7"/>
       <c r="J16" s="7"/>
       <c r="K16" s="9" t="n">
-        <v>295331</v>
-      </c>
-      <c r="L16" s="8"/>
+        <v>350379</v>
+      </c>
+      <c r="L16" s="8" t="s">
+        <v>47</v>
+      </c>
       <c r="M16" s="8"/>
       <c r="N16" s="8"/>
       <c r="O16" s="8"/>
@@ -2406,7 +2534,7 @@
         <v>10</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C17" s="5" t="n">
         <v>0</v>
@@ -2425,9 +2553,11 @@
       <c r="I17" s="7"/>
       <c r="J17" s="7"/>
       <c r="K17" s="9" t="n">
-        <v>325614</v>
-      </c>
-      <c r="L17" s="8"/>
+        <v>350377</v>
+      </c>
+      <c r="L17" s="8" t="s">
+        <v>49</v>
+      </c>
       <c r="M17" s="8"/>
       <c r="N17" s="8"/>
       <c r="O17" s="8"/>
@@ -2442,7 +2572,7 @@
         <v>11</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="C18" s="5" t="n">
         <v>0</v>
@@ -2461,9 +2591,11 @@
       <c r="I18" s="7"/>
       <c r="J18" s="7"/>
       <c r="K18" s="9" t="n">
-        <v>325605</v>
-      </c>
-      <c r="L18" s="8"/>
+        <v>350369</v>
+      </c>
+      <c r="L18" s="8" t="s">
+        <v>51</v>
+      </c>
       <c r="M18" s="8"/>
       <c r="N18" s="8"/>
       <c r="O18" s="8"/>
@@ -2478,7 +2610,7 @@
         <v>12</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="C19" s="5" t="n">
         <v>0</v>
@@ -2497,9 +2629,11 @@
       <c r="I19" s="7"/>
       <c r="J19" s="7"/>
       <c r="K19" s="5" t="n">
-        <v>325615</v>
-      </c>
-      <c r="L19" s="8"/>
+        <v>350361</v>
+      </c>
+      <c r="L19" s="8" t="s">
+        <v>53</v>
+      </c>
       <c r="M19" s="8"/>
       <c r="N19" s="8"/>
       <c r="O19" s="8"/>
@@ -2514,7 +2648,7 @@
         <v>13</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="C20" s="5" t="n">
         <v>0</v>
@@ -2533,9 +2667,11 @@
       <c r="I20" s="7"/>
       <c r="J20" s="7"/>
       <c r="K20" s="9" t="n">
-        <v>325602</v>
-      </c>
-      <c r="L20" s="8"/>
+        <v>350348</v>
+      </c>
+      <c r="L20" s="8" t="s">
+        <v>55</v>
+      </c>
       <c r="M20" s="8"/>
       <c r="N20" s="8"/>
       <c r="O20" s="8"/>
@@ -2550,7 +2686,7 @@
         <v>14</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="C21" s="5" t="n">
         <v>0</v>
@@ -2569,9 +2705,11 @@
       <c r="I21" s="7"/>
       <c r="J21" s="7"/>
       <c r="K21" s="5" t="n">
-        <v>325612</v>
-      </c>
-      <c r="L21" s="8"/>
+        <v>350373</v>
+      </c>
+      <c r="L21" s="8" t="s">
+        <v>57</v>
+      </c>
       <c r="M21" s="8"/>
       <c r="N21" s="8"/>
       <c r="O21" s="8"/>
@@ -2586,7 +2724,7 @@
         <v>15</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="C22" s="5" t="n">
         <v>0</v>
@@ -2605,9 +2743,11 @@
       <c r="I22" s="7"/>
       <c r="J22" s="7"/>
       <c r="K22" s="9" t="n">
-        <v>325610</v>
-      </c>
-      <c r="L22" s="8"/>
+        <v>350363</v>
+      </c>
+      <c r="L22" s="8" t="s">
+        <v>59</v>
+      </c>
       <c r="M22" s="8"/>
       <c r="N22" s="8"/>
       <c r="O22" s="8"/>
@@ -2622,7 +2762,7 @@
         <v>16</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="C23" s="10" t="n">
         <v>0</v>
@@ -2643,7 +2783,9 @@
       <c r="K23" s="10" t="n">
         <v>326706</v>
       </c>
-      <c r="L23" s="13"/>
+      <c r="L23" s="13" t="s">
+        <v>61</v>
+      </c>
       <c r="M23" s="13"/>
       <c r="N23" s="13"/>
       <c r="O23" s="13"/>
@@ -2658,7 +2800,7 @@
         <v>17</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="C24" s="10" t="n">
         <v>0</v>
@@ -2679,7 +2821,9 @@
       <c r="K24" s="10" t="n">
         <v>326704</v>
       </c>
-      <c r="L24" s="13"/>
+      <c r="L24" s="13" t="s">
+        <v>63</v>
+      </c>
       <c r="M24" s="13"/>
       <c r="N24" s="13"/>
       <c r="O24" s="13"/>
@@ -2694,7 +2838,7 @@
         <v>18</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="C25" s="10" t="n">
         <v>0</v>
@@ -2713,9 +2857,11 @@
       <c r="I25" s="12"/>
       <c r="J25" s="12"/>
       <c r="K25" s="10" t="n">
-        <v>326705</v>
-      </c>
-      <c r="L25" s="13"/>
+        <v>350347</v>
+      </c>
+      <c r="L25" s="13" t="s">
+        <v>65</v>
+      </c>
       <c r="M25" s="13"/>
       <c r="N25" s="13"/>
       <c r="O25" s="13"/>
@@ -2730,7 +2876,7 @@
         <v>19</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
       <c r="C26" s="10" t="n">
         <v>0</v>
@@ -2749,9 +2895,11 @@
       <c r="I26" s="12"/>
       <c r="J26" s="12"/>
       <c r="K26" s="10" t="n">
-        <v>294724</v>
-      </c>
-      <c r="L26" s="13"/>
+        <v>350345</v>
+      </c>
+      <c r="L26" s="13" t="s">
+        <v>67</v>
+      </c>
       <c r="M26" s="13"/>
       <c r="N26" s="13"/>
       <c r="O26" s="13"/>
@@ -2766,7 +2914,7 @@
         <v>20</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="C27" s="10" t="n">
         <v>0</v>
@@ -2787,7 +2935,9 @@
       <c r="K27" s="10" t="n">
         <v>326710</v>
       </c>
-      <c r="L27" s="13"/>
+      <c r="L27" s="13" t="s">
+        <v>69</v>
+      </c>
       <c r="M27" s="13"/>
       <c r="N27" s="13"/>
       <c r="O27" s="13"/>
@@ -2802,7 +2952,7 @@
         <v>21</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="C28" s="10" t="n">
         <v>0</v>
@@ -2823,7 +2973,9 @@
       <c r="K28" s="10" t="n">
         <v>327113</v>
       </c>
-      <c r="L28" s="13"/>
+      <c r="L28" s="13" t="s">
+        <v>71</v>
+      </c>
       <c r="M28" s="13"/>
       <c r="N28" s="13"/>
       <c r="O28" s="13"/>
@@ -2838,7 +2990,7 @@
         <v>22</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>56</v>
+        <v>72</v>
       </c>
       <c r="C29" s="10" t="n">
         <v>0</v>
@@ -2857,9 +3009,11 @@
       <c r="I29" s="12"/>
       <c r="J29" s="12"/>
       <c r="K29" s="10" t="n">
-        <v>326693</v>
-      </c>
-      <c r="L29" s="13"/>
+        <v>350352</v>
+      </c>
+      <c r="L29" s="13" t="s">
+        <v>73</v>
+      </c>
       <c r="M29" s="13"/>
       <c r="N29" s="13"/>
       <c r="O29" s="13"/>
@@ -2874,7 +3028,7 @@
         <v>23</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>57</v>
+        <v>74</v>
       </c>
       <c r="C30" s="10" t="n">
         <v>0</v>
@@ -2895,7 +3049,9 @@
       <c r="K30" s="10" t="n">
         <v>326698</v>
       </c>
-      <c r="L30" s="13"/>
+      <c r="L30" s="13" t="s">
+        <v>75</v>
+      </c>
       <c r="M30" s="13"/>
       <c r="N30" s="13"/>
       <c r="O30" s="13"/>
@@ -2910,7 +3066,7 @@
         <v>24</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>58</v>
+        <v>76</v>
       </c>
       <c r="C31" s="10" t="n">
         <v>0</v>
@@ -2929,9 +3085,11 @@
       <c r="I31" s="12"/>
       <c r="J31" s="12"/>
       <c r="K31" s="10" t="n">
-        <v>326699</v>
-      </c>
-      <c r="L31" s="13"/>
+        <v>350346</v>
+      </c>
+      <c r="L31" s="13" t="s">
+        <v>77</v>
+      </c>
       <c r="M31" s="13"/>
       <c r="N31" s="13"/>
       <c r="O31" s="13"/>
@@ -2946,7 +3104,7 @@
         <v>25</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>59</v>
+        <v>78</v>
       </c>
       <c r="C32" s="10" t="n">
         <v>0</v>
@@ -2967,7 +3125,9 @@
       <c r="K32" s="10" t="n">
         <v>326712</v>
       </c>
-      <c r="L32" s="13"/>
+      <c r="L32" s="13" t="s">
+        <v>79</v>
+      </c>
       <c r="M32" s="13"/>
       <c r="N32" s="13"/>
       <c r="O32" s="13"/>
@@ -2982,7 +3142,7 @@
         <v>26</v>
       </c>
       <c r="B33" s="15" t="s">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="C33" s="14" t="n">
         <v>0</v>
@@ -3003,7 +3163,9 @@
       <c r="K33" s="14" t="n">
         <v>327119</v>
       </c>
-      <c r="L33" s="18"/>
+      <c r="L33" s="18" t="s">
+        <v>81</v>
+      </c>
       <c r="M33" s="18"/>
       <c r="N33" s="18"/>
       <c r="O33" s="18"/>
@@ -3018,7 +3180,7 @@
         <v>27</v>
       </c>
       <c r="B34" s="15" t="s">
-        <v>61</v>
+        <v>82</v>
       </c>
       <c r="C34" s="14" t="n">
         <v>0</v>
@@ -3037,9 +3199,11 @@
       <c r="I34" s="17"/>
       <c r="J34" s="17"/>
       <c r="K34" s="14" t="n">
-        <v>294753</v>
-      </c>
-      <c r="L34" s="18"/>
+        <v>350354</v>
+      </c>
+      <c r="L34" s="18" t="s">
+        <v>83</v>
+      </c>
       <c r="M34" s="18"/>
       <c r="N34" s="18"/>
       <c r="O34" s="18"/>
@@ -3054,7 +3218,7 @@
         <v>28</v>
       </c>
       <c r="B35" s="15" t="s">
-        <v>62</v>
+        <v>84</v>
       </c>
       <c r="C35" s="14" t="n">
         <v>0</v>
@@ -3073,9 +3237,11 @@
       <c r="I35" s="17"/>
       <c r="J35" s="17"/>
       <c r="K35" s="14" t="n">
-        <v>327136</v>
-      </c>
-      <c r="L35" s="18"/>
+        <v>350337</v>
+      </c>
+      <c r="L35" s="18" t="s">
+        <v>85</v>
+      </c>
       <c r="M35" s="18"/>
       <c r="N35" s="18"/>
       <c r="O35" s="18"/>
@@ -3090,7 +3256,7 @@
         <v>29</v>
       </c>
       <c r="B36" s="15" t="s">
-        <v>63</v>
+        <v>86</v>
       </c>
       <c r="C36" s="14" t="n">
         <v>0</v>
@@ -3111,7 +3277,9 @@
       <c r="K36" s="14" t="n">
         <v>327101</v>
       </c>
-      <c r="L36" s="18"/>
+      <c r="L36" s="18" t="s">
+        <v>87</v>
+      </c>
       <c r="M36" s="18"/>
       <c r="N36" s="18"/>
       <c r="O36" s="18"/>
@@ -3126,7 +3294,7 @@
         <v>30</v>
       </c>
       <c r="B37" s="15" t="s">
-        <v>64</v>
+        <v>88</v>
       </c>
       <c r="C37" s="14" t="n">
         <v>0</v>
@@ -3145,9 +3313,11 @@
       <c r="I37" s="17"/>
       <c r="J37" s="17"/>
       <c r="K37" s="14" t="n">
-        <v>294753</v>
-      </c>
-      <c r="L37" s="18"/>
+        <v>327133</v>
+      </c>
+      <c r="L37" s="18" t="s">
+        <v>89</v>
+      </c>
       <c r="M37" s="18"/>
       <c r="N37" s="18"/>
       <c r="O37" s="18"/>
@@ -3162,7 +3332,7 @@
         <v>31</v>
       </c>
       <c r="B38" s="15" t="s">
-        <v>65</v>
+        <v>90</v>
       </c>
       <c r="C38" s="14" t="n">
         <v>0</v>
@@ -3183,7 +3353,9 @@
       <c r="K38" s="14" t="n">
         <v>327099</v>
       </c>
-      <c r="L38" s="18"/>
+      <c r="L38" s="18" t="s">
+        <v>91</v>
+      </c>
       <c r="M38" s="18"/>
       <c r="N38" s="18"/>
       <c r="O38" s="18"/>
@@ -3198,7 +3370,7 @@
         <v>32</v>
       </c>
       <c r="B39" s="15" t="s">
-        <v>66</v>
+        <v>92</v>
       </c>
       <c r="C39" s="14" t="n">
         <v>0</v>
@@ -3219,7 +3391,9 @@
       <c r="K39" s="14" t="n">
         <v>327118</v>
       </c>
-      <c r="L39" s="18"/>
+      <c r="L39" s="18" t="s">
+        <v>93</v>
+      </c>
       <c r="M39" s="18"/>
       <c r="N39" s="18"/>
       <c r="O39" s="18"/>
@@ -3234,7 +3408,7 @@
         <v>33</v>
       </c>
       <c r="B40" s="15" t="s">
-        <v>67</v>
+        <v>94</v>
       </c>
       <c r="C40" s="14" t="n">
         <v>0</v>
@@ -3253,9 +3427,11 @@
       <c r="I40" s="17"/>
       <c r="J40" s="17"/>
       <c r="K40" s="14" t="n">
-        <v>327099</v>
-      </c>
-      <c r="L40" s="18"/>
+        <v>350410</v>
+      </c>
+      <c r="L40" s="18" t="s">
+        <v>95</v>
+      </c>
       <c r="M40" s="18"/>
       <c r="N40" s="18"/>
       <c r="O40" s="18"/>
@@ -3270,7 +3446,7 @@
         <v>34</v>
       </c>
       <c r="B41" s="15" t="s">
-        <v>68</v>
+        <v>96</v>
       </c>
       <c r="C41" s="14" t="n">
         <v>0</v>
@@ -3291,7 +3467,9 @@
       <c r="K41" s="14" t="n">
         <v>327126</v>
       </c>
-      <c r="L41" s="18"/>
+      <c r="L41" s="18" t="s">
+        <v>97</v>
+      </c>
       <c r="M41" s="18"/>
       <c r="N41" s="18"/>
       <c r="O41" s="18"/>
@@ -3306,7 +3484,7 @@
         <v>35</v>
       </c>
       <c r="B42" s="15" t="s">
-        <v>69</v>
+        <v>98</v>
       </c>
       <c r="C42" s="14" t="n">
         <v>0</v>
@@ -3327,7 +3505,9 @@
       <c r="K42" s="14" t="n">
         <v>327104</v>
       </c>
-      <c r="L42" s="18"/>
+      <c r="L42" s="18" t="s">
+        <v>99</v>
+      </c>
       <c r="M42" s="18"/>
       <c r="N42" s="18"/>
       <c r="O42" s="18"/>
@@ -3342,7 +3522,7 @@
         <v>36</v>
       </c>
       <c r="B43" s="20" t="s">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="C43" s="19" t="n">
         <v>1</v>
@@ -3354,7 +3534,7 @@
         <v>1</v>
       </c>
       <c r="F43" s="21" t="s">
-        <v>71</v>
+        <v>101</v>
       </c>
       <c r="G43" s="22" t="n">
         <v>0.3</v>
@@ -3382,7 +3562,7 @@
         <v>37</v>
       </c>
       <c r="B44" s="20" t="s">
-        <v>72</v>
+        <v>102</v>
       </c>
       <c r="C44" s="19" t="n">
         <v>0</v>
@@ -3403,7 +3583,9 @@
       <c r="K44" s="19" t="n">
         <v>327083</v>
       </c>
-      <c r="L44" s="23"/>
+      <c r="L44" s="23" t="s">
+        <v>103</v>
+      </c>
       <c r="M44" s="23"/>
       <c r="N44" s="23"/>
       <c r="O44" s="23"/>
@@ -3418,7 +3600,7 @@
         <v>38</v>
       </c>
       <c r="B45" s="20" t="s">
-        <v>73</v>
+        <v>104</v>
       </c>
       <c r="C45" s="19" t="n">
         <v>0</v>
@@ -3439,7 +3621,9 @@
       <c r="K45" s="19" t="n">
         <v>327089</v>
       </c>
-      <c r="L45" s="23"/>
+      <c r="L45" s="23" t="s">
+        <v>105</v>
+      </c>
       <c r="M45" s="23"/>
       <c r="N45" s="23"/>
       <c r="O45" s="23"/>
@@ -3454,7 +3638,7 @@
         <v>39</v>
       </c>
       <c r="B46" s="20" t="s">
-        <v>74</v>
+        <v>106</v>
       </c>
       <c r="C46" s="19" t="n">
         <v>0</v>
@@ -3473,9 +3657,11 @@
       <c r="I46" s="22"/>
       <c r="J46" s="22"/>
       <c r="K46" s="19" t="n">
-        <v>295345</v>
-      </c>
-      <c r="L46" s="23"/>
+        <v>350406</v>
+      </c>
+      <c r="L46" s="23" t="s">
+        <v>107</v>
+      </c>
       <c r="M46" s="23"/>
       <c r="N46" s="23"/>
       <c r="O46" s="23"/>
@@ -3490,7 +3676,7 @@
         <v>40</v>
       </c>
       <c r="B47" s="20" t="s">
-        <v>75</v>
+        <v>108</v>
       </c>
       <c r="C47" s="19" t="n">
         <v>0</v>
@@ -3511,7 +3697,9 @@
       <c r="K47" s="19" t="n">
         <v>327088</v>
       </c>
-      <c r="L47" s="23"/>
+      <c r="L47" s="23" t="s">
+        <v>109</v>
+      </c>
       <c r="M47" s="23"/>
       <c r="N47" s="23"/>
       <c r="O47" s="23"/>
@@ -3526,7 +3714,7 @@
         <v>41</v>
       </c>
       <c r="B48" s="20" t="s">
-        <v>76</v>
+        <v>110</v>
       </c>
       <c r="C48" s="19" t="n">
         <v>0</v>
@@ -3547,7 +3735,9 @@
       <c r="K48" s="19" t="n">
         <v>327087</v>
       </c>
-      <c r="L48" s="23"/>
+      <c r="L48" s="23" t="s">
+        <v>111</v>
+      </c>
       <c r="M48" s="23"/>
       <c r="N48" s="23"/>
       <c r="O48" s="23"/>
@@ -3562,7 +3752,7 @@
         <v>42</v>
       </c>
       <c r="B49" s="20" t="s">
-        <v>77</v>
+        <v>112</v>
       </c>
       <c r="C49" s="19" t="n">
         <v>0</v>
@@ -3581,9 +3771,11 @@
       <c r="I49" s="22"/>
       <c r="J49" s="22"/>
       <c r="K49" s="19" t="n">
-        <v>327170</v>
-      </c>
-      <c r="L49" s="23"/>
+        <v>350375</v>
+      </c>
+      <c r="L49" s="23" t="s">
+        <v>113</v>
+      </c>
       <c r="M49" s="23"/>
       <c r="N49" s="23"/>
       <c r="O49" s="23"/>
@@ -3598,7 +3790,7 @@
         <v>43</v>
       </c>
       <c r="B50" s="20" t="s">
-        <v>78</v>
+        <v>114</v>
       </c>
       <c r="C50" s="19" t="n">
         <v>0</v>
@@ -3617,9 +3809,11 @@
       <c r="I50" s="22"/>
       <c r="J50" s="22"/>
       <c r="K50" s="19" t="n">
-        <v>327094</v>
-      </c>
-      <c r="L50" s="23"/>
+        <v>350391</v>
+      </c>
+      <c r="L50" s="23" t="s">
+        <v>115</v>
+      </c>
       <c r="M50" s="23"/>
       <c r="N50" s="23"/>
       <c r="O50" s="23"/>
@@ -3634,7 +3828,7 @@
         <v>44</v>
       </c>
       <c r="B51" s="20" t="s">
-        <v>79</v>
+        <v>116</v>
       </c>
       <c r="C51" s="19" t="n">
         <v>0</v>
@@ -3655,7 +3849,9 @@
       <c r="K51" s="19" t="n">
         <v>327171</v>
       </c>
-      <c r="L51" s="23"/>
+      <c r="L51" s="23" t="s">
+        <v>117</v>
+      </c>
       <c r="M51" s="23"/>
       <c r="N51" s="23"/>
       <c r="O51" s="23"/>
@@ -3670,7 +3866,7 @@
         <v>45</v>
       </c>
       <c r="B52" s="20" t="s">
-        <v>80</v>
+        <v>118</v>
       </c>
       <c r="C52" s="19" t="n">
         <v>0</v>
@@ -3689,9 +3885,11 @@
       <c r="I52" s="22"/>
       <c r="J52" s="22"/>
       <c r="K52" s="19" t="n">
-        <v>327097</v>
-      </c>
-      <c r="L52" s="23"/>
+        <v>350386</v>
+      </c>
+      <c r="L52" s="23" t="s">
+        <v>119</v>
+      </c>
       <c r="M52" s="23"/>
       <c r="N52" s="23"/>
       <c r="O52" s="23"/>
@@ -3706,7 +3904,7 @@
         <v>46</v>
       </c>
       <c r="B53" s="20" t="s">
-        <v>81</v>
+        <v>120</v>
       </c>
       <c r="C53" s="19" t="n">
         <v>0</v>
@@ -3727,7 +3925,9 @@
       <c r="K53" s="19" t="n">
         <v>327100</v>
       </c>
-      <c r="L53" s="23"/>
+      <c r="L53" s="23" t="s">
+        <v>121</v>
+      </c>
       <c r="M53" s="23"/>
       <c r="N53" s="23"/>
       <c r="O53" s="23"/>
@@ -3742,7 +3942,7 @@
         <v>47</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>82</v>
+        <v>122</v>
       </c>
       <c r="C54" s="5" t="n">
         <v>1</v>
@@ -3754,7 +3954,7 @@
         <v>1</v>
       </c>
       <c r="F54" s="25" t="s">
-        <v>83</v>
+        <v>123</v>
       </c>
       <c r="G54" s="7"/>
       <c r="H54" s="7"/>
@@ -3778,7 +3978,7 @@
         <v>48</v>
       </c>
       <c r="B55" s="11" t="s">
-        <v>84</v>
+        <v>124</v>
       </c>
       <c r="C55" s="10" t="n">
         <v>1</v>
@@ -3790,7 +3990,7 @@
         <v>1</v>
       </c>
       <c r="F55" s="26" t="s">
-        <v>85</v>
+        <v>125</v>
       </c>
       <c r="G55" s="12"/>
       <c r="H55" s="12"/>
@@ -3814,7 +4014,7 @@
         <v>49</v>
       </c>
       <c r="B56" s="15" t="s">
-        <v>86</v>
+        <v>126</v>
       </c>
       <c r="C56" s="14" t="n">
         <v>1</v>
@@ -3826,7 +4026,7 @@
         <v>1</v>
       </c>
       <c r="F56" s="27" t="s">
-        <v>87</v>
+        <v>127</v>
       </c>
       <c r="G56" s="17"/>
       <c r="H56" s="17"/>
@@ -3850,7 +4050,7 @@
         <v>50</v>
       </c>
       <c r="B57" s="20" t="s">
-        <v>88</v>
+        <v>128</v>
       </c>
       <c r="C57" s="19" t="n">
         <v>1</v>
@@ -3862,7 +4062,7 @@
         <v>1</v>
       </c>
       <c r="F57" s="21" t="s">
-        <v>89</v>
+        <v>129</v>
       </c>
       <c r="G57" s="22"/>
       <c r="H57" s="22"/>

</xml_diff>